<commit_message>
from roar; yield tests
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP/compiled_results.xlsx
+++ b/application/output_max_withoutMP/compiled_results.xlsx
@@ -616,25 +616,25 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.8138221659621</v>
+        <v>17.81382214929636</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5695516945319341</v>
+        <v>0.5695516939990893</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
       </c>
       <c r="H2" t="n">
-        <v>17.03005393819904</v>
+        <v>10.33377596184603</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5444926971935806</v>
+        <v>0.3303962257593862</v>
       </c>
       <c r="J2" t="n">
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9560022425024171</v>
+        <v>0.5800987500177894</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -654,11 +654,11 @@
       </c>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="n">
-        <v>17.03005393819904</v>
+        <v>10.33377596184603</v>
       </c>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
-        <v>0.5444926971935806</v>
+        <v>0.3303962257593862</v>
       </c>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
@@ -687,25 +687,25 @@
         <v>122.16</v>
       </c>
       <c r="E3" t="n">
-        <v>6.941370065782265</v>
+        <v>6.94137006466926</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3563056215255053</v>
+        <v>0.356305621468374</v>
       </c>
       <c r="G3" t="n">
         <v>-13.21</v>
       </c>
       <c r="H3" t="n">
-        <v>6.503098170437087</v>
+        <v>3.765885265022366</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3338088033774693</v>
+        <v>0.1933056554010884</v>
       </c>
       <c r="J3" t="n">
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9368608947237009</v>
+        <v>0.5425276609570595</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
@@ -725,11 +725,11 @@
       </c>
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="n">
-        <v>6.503098170437087</v>
+        <v>3.765885265022366</v>
       </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="n">
-        <v>0.3338088033774693</v>
+        <v>0.1933056554010884</v>
       </c>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
@@ -758,25 +758,25 @@
         <v>90.08</v>
       </c>
       <c r="E4" t="n">
-        <v>20.06614450050855</v>
+        <v>20.06614449001378</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7595227111546687</v>
+        <v>0.7595227107574315</v>
       </c>
       <c r="G4" t="n">
         <v>-13.21</v>
       </c>
       <c r="H4" t="n">
-        <v>15.22378166356998</v>
+        <v>4.789907146774331</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5762346584740462</v>
+        <v>0.1813025547685536</v>
       </c>
       <c r="J4" t="n">
         <v>-13.21</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7586799578356547</v>
+        <v>0.2387059033267751</v>
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
@@ -796,11 +796,11 @@
       </c>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="n">
-        <v>15.22378166356998</v>
+        <v>4.789907146774331</v>
       </c>
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="n">
-        <v>0.5762346584740462</v>
+        <v>0.1813025547685536</v>
       </c>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr"/>
@@ -829,25 +829,25 @@
         <v>90.08</v>
       </c>
       <c r="E5" t="n">
-        <v>22.34089255192158</v>
+        <v>22.34089253733244</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8456240948638927</v>
+        <v>0.8456240943116801</v>
       </c>
       <c r="G5" t="n">
         <v>-13.21</v>
       </c>
       <c r="H5" t="n">
-        <v>20.4935941299499</v>
+        <v>8.273785303551145</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7757020873884602</v>
+        <v>0.3131706663980993</v>
       </c>
       <c r="J5" t="n">
         <v>-13.21</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9173131325134642</v>
+        <v>0.3703426481160208</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
@@ -867,11 +867,11 @@
       </c>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="n">
-        <v>20.4935941299499</v>
+        <v>8.273785303551145</v>
       </c>
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="n">
-        <v>0.7757020873884602</v>
+        <v>0.3131706663980993</v>
       </c>
       <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="inlineStr"/>
@@ -900,25 +900,25 @@
         <v>90.08</v>
       </c>
       <c r="E6" t="n">
-        <v>20.06614450050855</v>
+        <v>20.06614449001378</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7595227111546687</v>
+        <v>0.7595227107574315</v>
       </c>
       <c r="G6" t="n">
         <v>-13.21</v>
       </c>
       <c r="H6" t="n">
-        <v>15.22378166356998</v>
+        <v>4.789907146774331</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5762346584740462</v>
+        <v>0.1813025547685536</v>
       </c>
       <c r="J6" t="n">
         <v>-13.21</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7586799578356547</v>
+        <v>0.2387059033267751</v>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
@@ -938,11 +938,11 @@
       </c>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="n">
-        <v>15.22378166356998</v>
+        <v>4.789907146774331</v>
       </c>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="n">
-        <v>0.5762346584740462</v>
+        <v>0.1813025547685536</v>
       </c>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="inlineStr"/>
@@ -971,25 +971,25 @@
         <v>90.08</v>
       </c>
       <c r="E7" t="n">
-        <v>22.34089255192158</v>
+        <v>22.34089253733244</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8456240948638927</v>
+        <v>0.8456240943116801</v>
       </c>
       <c r="G7" t="n">
         <v>-13.21</v>
       </c>
       <c r="H7" t="n">
-        <v>20.4935941299499</v>
+        <v>8.273785303551145</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7757020873884602</v>
+        <v>0.3131706663980993</v>
       </c>
       <c r="J7" t="n">
         <v>-13.21</v>
       </c>
       <c r="K7" t="n">
-        <v>0.9173131325134642</v>
+        <v>0.3703426481160208</v>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
@@ -1009,11 +1009,11 @@
       </c>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="n">
-        <v>20.4935941299499</v>
+        <v>8.273785303551145</v>
       </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="n">
-        <v>0.7757020873884602</v>
+        <v>0.3131706663980993</v>
       </c>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
@@ -1042,25 +1042,25 @@
         <v>137.11</v>
       </c>
       <c r="E8" t="n">
-        <v>9.055951953675855</v>
+        <v>9.055951945825333</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5217370668225551</v>
+        <v>0.521737066370266</v>
       </c>
       <c r="G8" t="n">
         <v>-13.21</v>
       </c>
       <c r="H8" t="n">
-        <v>7.956152383411257</v>
+        <v>3.201830994039559</v>
       </c>
       <c r="I8" t="n">
-        <v>0.458374738398358</v>
+        <v>0.1844658540412944</v>
       </c>
       <c r="J8" t="n">
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>0.8785550568410221</v>
+        <v>0.3535609523099952</v>
       </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
@@ -1080,11 +1080,11 @@
       </c>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="n">
-        <v>7.956152383411257</v>
+        <v>3.201830994039559</v>
       </c>
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="n">
-        <v>0.458374738398358</v>
+        <v>0.1844658540412944</v>
       </c>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
@@ -1113,25 +1113,25 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.844697658781199</v>
+        <v>2.844697657836357</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2800995812806286</v>
+        <v>0.2800995811875959</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
       </c>
       <c r="H9" t="n">
-        <v>2.398459109383042</v>
+        <v>1.268691931624992</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2361612631075644</v>
+        <v>0.1249201572354529</v>
       </c>
       <c r="J9" t="n">
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.8431332243619357</v>
+        <v>0.445984805495971</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1151,11 +1151,11 @@
       </c>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="n">
-        <v>2.398459109383042</v>
+        <v>1.268691931624992</v>
       </c>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
-        <v>0.2361612631075644</v>
+        <v>0.1249201572354529</v>
       </c>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="inlineStr"/>
@@ -1184,25 +1184,25 @@
         <v>90.12</v>
       </c>
       <c r="E10" t="n">
-        <v>12.8944378515529</v>
+        <v>12.89443785011522</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4882834990656963</v>
+        <v>0.4882834990112545</v>
       </c>
       <c r="G10" t="n">
         <v>-13.21</v>
       </c>
       <c r="H10" t="n">
-        <v>12.31090878407757</v>
+        <v>12.86101832859688</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4661865594275652</v>
+        <v>0.48701797653622</v>
       </c>
       <c r="J10" t="n">
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>0.95474567606644</v>
+        <v>0.9974082219087946</v>
       </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
@@ -1222,11 +1222,11 @@
       </c>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="n">
-        <v>12.31090878407757</v>
+        <v>12.86101832859688</v>
       </c>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
-        <v>0.4661865594275652</v>
+        <v>0.48701797653622</v>
       </c>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="inlineStr"/>
@@ -1255,25 +1255,25 @@
         <v>74.12</v>
       </c>
       <c r="E11" t="n">
-        <v>11.1978729796163</v>
+        <v>11.19787297467806</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3487541620918865</v>
+        <v>0.3487541619380868</v>
       </c>
       <c r="G11" t="n">
         <v>-13.21</v>
       </c>
       <c r="H11" t="n">
-        <v>10.06059178759377</v>
+        <v>8.787635674310453</v>
       </c>
       <c r="I11" t="n">
-        <v>0.3133339041635572</v>
+        <v>0.2736880943319939</v>
       </c>
       <c r="J11" t="n">
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>0.898437748481989</v>
+        <v>0.7847593640490544</v>
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -1293,11 +1293,11 @@
       </c>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="n">
-        <v>10.06059178759377</v>
+        <v>8.787635674310453</v>
       </c>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
-        <v>0.3133339041635572</v>
+        <v>0.2736880943319939</v>
       </c>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="inlineStr"/>
@@ -1326,25 +1326,25 @@
         <v>146.1</v>
       </c>
       <c r="E12" t="n">
-        <v>12.48937108880212</v>
+        <v>12.48937108880217</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7667243171293724</v>
+        <v>0.7667243171293756</v>
       </c>
       <c r="G12" t="n">
         <v>-13.21</v>
       </c>
       <c r="H12" t="n">
-        <v>11.49508371910139</v>
+        <v>4.983742289914067</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7056848701353072</v>
+        <v>0.3059526678176101</v>
       </c>
       <c r="J12" t="n">
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>0.9203893164330593</v>
+        <v>0.3990386909379636</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1364,11 +1364,11 @@
       </c>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="n">
-        <v>11.49508371910139</v>
+        <v>4.983742289914067</v>
       </c>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
-        <v>0.7056848701353072</v>
+        <v>0.3059526678176101</v>
       </c>
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="inlineStr"/>
@@ -1397,25 +1397,25 @@
         <v>163.15</v>
       </c>
       <c r="E13" t="n">
-        <v>7.096204244674719</v>
+        <v>7.096204240677997</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4864762434751352</v>
+        <v>0.4864762432011422</v>
       </c>
       <c r="G13" t="n">
         <v>-13.21</v>
       </c>
       <c r="H13" t="n">
-        <v>6.448760769918064</v>
+        <v>3.08763752503665</v>
       </c>
       <c r="I13" t="n">
-        <v>0.4420911245295426</v>
+        <v>0.211671233324478</v>
       </c>
       <c r="J13" t="n">
         <v>-13.21</v>
       </c>
       <c r="K13" t="n">
-        <v>0.9087620011441294</v>
+        <v>0.4351111411558873</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
@@ -1435,11 +1435,11 @@
       </c>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="n">
-        <v>6.448760769918064</v>
+        <v>3.08763752503665</v>
       </c>
       <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="n">
-        <v>0.4420911245295426</v>
+        <v>0.211671233324478</v>
       </c>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="inlineStr"/>
@@ -1468,25 +1468,25 @@
         <v>256.4</v>
       </c>
       <c r="E14" t="n">
-        <v>2.76196014519293</v>
+        <v>2.761960143974937</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2975663925932656</v>
+        <v>0.2975663924620421</v>
       </c>
       <c r="G14" t="n">
         <v>-13.21</v>
       </c>
       <c r="H14" t="n">
-        <v>2.125096075944671</v>
+        <v>0.716460988511289</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2289523164675456</v>
+        <v>0.07718964089911483</v>
       </c>
       <c r="J14" t="n">
         <v>-13.21</v>
       </c>
       <c r="K14" t="n">
-        <v>0.7694159090757724</v>
+        <v>0.259403087359609</v>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
@@ -1506,11 +1506,11 @@
       </c>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="n">
-        <v>2.125096075944671</v>
+        <v>0.716460988511289</v>
       </c>
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="n">
-        <v>0.2289523164675456</v>
+        <v>0.07718964089911483</v>
       </c>
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="inlineStr"/>
@@ -1539,25 +1539,25 @@
         <v>242.44</v>
       </c>
       <c r="E15" t="n">
-        <v>2.677177423438271</v>
+        <v>2.677177422360339</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2727280963018923</v>
+        <v>0.2727280961920816</v>
       </c>
       <c r="G15" t="n">
         <v>-13.21</v>
       </c>
       <c r="H15" t="n">
-        <v>2.097690532032536</v>
+        <v>0.7283461481432379</v>
       </c>
       <c r="I15" t="n">
-        <v>0.2136948938920141</v>
+        <v>0.07419771909506445</v>
       </c>
       <c r="J15" t="n">
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.7835455781404632</v>
+        <v>0.2720574819061077</v>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
@@ -1577,11 +1577,11 @@
       </c>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="n">
-        <v>2.097690532032536</v>
+        <v>0.7283461481432379</v>
       </c>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="n">
-        <v>0.2136948938920141</v>
+        <v>0.07419771909506445</v>
       </c>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
@@ -1610,25 +1610,25 @@
         <v>74.12</v>
       </c>
       <c r="E16" t="n">
-        <v>12.52385380260007</v>
+        <v>12.52385380260009</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3900514094987295</v>
+        <v>0.39005140949873</v>
       </c>
       <c r="G16" t="n">
         <v>-13.21</v>
       </c>
       <c r="H16" t="n">
-        <v>11.8302192595611</v>
+        <v>12.3642424889837</v>
       </c>
       <c r="I16" t="n">
-        <v>0.3684483841477635</v>
+        <v>0.385080366333479</v>
       </c>
       <c r="J16" t="n">
         <v>-13.21</v>
       </c>
       <c r="K16" t="n">
-        <v>0.9446149281226062</v>
+        <v>0.9872554154550053</v>
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
@@ -1648,11 +1648,11 @@
       </c>
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="n">
-        <v>11.8302192595611</v>
+        <v>12.3642424889837</v>
       </c>
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="n">
-        <v>0.3684483841477635</v>
+        <v>0.385080366333479</v>
       </c>
       <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="inlineStr"/>
@@ -1681,25 +1681,25 @@
         <v>89.06999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>24.24659127198081</v>
+        <v>24.24659125876742</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9074664874911968</v>
+        <v>0.9074664869966653</v>
       </c>
       <c r="G17" t="n">
         <v>-13.21</v>
       </c>
       <c r="H17" t="n">
-        <v>23.15800090048398</v>
+        <v>21.15294223104609</v>
       </c>
       <c r="I17" t="n">
-        <v>0.8667242953348701</v>
+        <v>0.7916818480251235</v>
       </c>
       <c r="J17" t="n">
         <v>-13.21</v>
       </c>
       <c r="K17" t="n">
-        <v>0.9551033644570571</v>
+        <v>0.872408909165626</v>
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
@@ -1719,11 +1719,11 @@
       </c>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="n">
-        <v>23.15800090048398</v>
+        <v>21.15294223104609</v>
       </c>
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="n">
-        <v>0.8667242953348701</v>
+        <v>0.7916818480251235</v>
       </c>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
@@ -1752,25 +1752,25 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>10.42241535589292</v>
+        <v>10.42241535083183</v>
       </c>
       <c r="F18" t="n">
-        <v>0.6135132742837609</v>
+        <v>0.6135132739858409</v>
       </c>
       <c r="G18" t="n">
         <v>-13.21</v>
       </c>
       <c r="H18" t="n">
-        <v>9.619565848243479</v>
+        <v>4.807363077610548</v>
       </c>
       <c r="I18" t="n">
-        <v>0.5662537079187897</v>
+        <v>0.2829844102066129</v>
       </c>
       <c r="J18" t="n">
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>0.9229689587073012</v>
+        <v>0.4612523024451201</v>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
@@ -1790,11 +1790,11 @@
       </c>
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="n">
-        <v>9.619565848243479</v>
+        <v>4.807363077610548</v>
       </c>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="n">
-        <v>0.5662537079187897</v>
+        <v>0.2829844102066129</v>
       </c>
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="inlineStr"/>
@@ -1823,25 +1823,25 @@
         <v>272.25</v>
       </c>
       <c r="E19" t="n">
-        <v>3.969093041860369</v>
+        <v>3.969093040440947</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4540541189672314</v>
+        <v>0.4540541188048531</v>
       </c>
       <c r="G19" t="n">
         <v>-13.21</v>
       </c>
       <c r="H19" t="n">
-        <v>3.183054426087371</v>
+        <v>1.076926979514537</v>
       </c>
       <c r="I19" t="n">
-        <v>0.3641333064806223</v>
+        <v>0.1231976992523011</v>
       </c>
       <c r="J19" t="n">
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.8019601436693529</v>
+        <v>0.2713282275174118</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1861,11 +1861,11 @@
       </c>
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="n">
-        <v>3.183054426087371</v>
+        <v>1.076926979514537</v>
       </c>
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="n">
-        <v>0.3641333064806223</v>
+        <v>0.1231976992523011</v>
       </c>
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="inlineStr"/>
@@ -1894,10 +1894,10 @@
         <v>268.5</v>
       </c>
       <c r="E20" t="n">
-        <v>0.09996363129559631</v>
+        <v>0.09996363102997334</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2355252494907961</v>
+        <v>0.2355252488649593</v>
       </c>
       <c r="G20" t="n">
         <v>-0.332925</v>
@@ -1973,10 +1973,10 @@
         <v>242.44</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1141673731007368</v>
+        <v>0.114167372765945</v>
       </c>
       <c r="F21" t="n">
-        <v>0.242883181049906</v>
+        <v>0.2428831803376595</v>
       </c>
       <c r="G21" t="n">
         <v>-0.332925</v>
@@ -2048,25 +2048,25 @@
         <v>103.1</v>
       </c>
       <c r="E22" t="n">
-        <v>12.48937108880207</v>
+        <v>12.48937108880214</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5410628137990281</v>
+        <v>0.5410628137990309</v>
       </c>
       <c r="G22" t="n">
         <v>-13.21</v>
       </c>
       <c r="H22" t="n">
-        <v>11.37822043193668</v>
+        <v>4.768756988393707</v>
       </c>
       <c r="I22" t="n">
-        <v>0.4929256981121332</v>
+        <v>0.2065914333170446</v>
       </c>
       <c r="J22" t="n">
         <v>-13.21</v>
       </c>
       <c r="K22" t="n">
-        <v>0.9110322970656509</v>
+        <v>0.3818252299885087</v>
       </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
@@ -2086,11 +2086,11 @@
       </c>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="n">
-        <v>11.37822043193668</v>
+        <v>4.768756988393707</v>
       </c>
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="n">
-        <v>0.4929256981121332</v>
+        <v>0.2065914333170446</v>
       </c>
       <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="inlineStr"/>
@@ -2119,25 +2119,25 @@
         <v>329.4</v>
       </c>
       <c r="E23" t="n">
-        <v>2.511143879318773</v>
+        <v>2.511143877685606</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3475710880865164</v>
+        <v>0.3475710878604674</v>
       </c>
       <c r="G23" t="n">
         <v>-13.21</v>
       </c>
       <c r="H23" t="n">
-        <v>1.612900652995342</v>
+        <v>0.491953794688782</v>
       </c>
       <c r="I23" t="n">
-        <v>0.2232439325974119</v>
+        <v>0.06809204248171426</v>
       </c>
       <c r="J23" t="n">
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.6422971882570471</v>
+        <v>0.1959082468592723</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2157,11 +2157,11 @@
       </c>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="n">
-        <v>1.612900652995342</v>
+        <v>0.491953794688782</v>
       </c>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="n">
-        <v>0.2232439325974119</v>
+        <v>0.06809204248171426</v>
       </c>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
@@ -2190,25 +2190,25 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>3.969093042542851</v>
+        <v>3.969093040440451</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3806549573219487</v>
+        <v>0.3806549571203185</v>
       </c>
       <c r="G24" t="n">
         <v>-13.21</v>
       </c>
       <c r="H24" t="n">
-        <v>3.183054425983536</v>
+        <v>1.076921922608241</v>
       </c>
       <c r="I24" t="n">
-        <v>0.3052701041999122</v>
+        <v>0.1032819498297476</v>
       </c>
       <c r="J24" t="n">
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.8019601435052957</v>
+        <v>0.2713269534464565</v>
       </c>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
@@ -2228,11 +2228,11 @@
       </c>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="n">
-        <v>3.183054425983536</v>
+        <v>1.076921922608241</v>
       </c>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="n">
-        <v>0.3052701041999122</v>
+        <v>0.1032819498297476</v>
       </c>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="inlineStr"/>
@@ -2261,25 +2261,25 @@
         <v>246.3</v>
       </c>
       <c r="E25" t="n">
-        <v>2.957467003591014</v>
+        <v>2.957467002868275</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3060784627519413</v>
+        <v>0.3060784626771426</v>
       </c>
       <c r="G25" t="n">
         <v>-13.21</v>
       </c>
       <c r="H25" t="n">
-        <v>2.49126643275709</v>
+        <v>1.323884235524466</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2578297573964248</v>
+        <v>0.1370133466168315</v>
       </c>
       <c r="J25" t="n">
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.8423649121806416</v>
+        <v>0.4476412532212557</v>
       </c>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
@@ -2299,11 +2299,11 @@
       </c>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="n">
-        <v>2.49126643275709</v>
+        <v>1.323884235524466</v>
       </c>
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="n">
-        <v>0.2578297573964248</v>
+        <v>0.1370133466168315</v>
       </c>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="inlineStr"/>
@@ -2332,25 +2332,25 @@
         <v>174.15</v>
       </c>
       <c r="E26" t="n">
-        <v>9.725652210493044</v>
+        <v>9.725652204072677</v>
       </c>
       <c r="F26" t="n">
-        <v>0.711689675683952</v>
+        <v>0.7116896752141317</v>
       </c>
       <c r="G26" t="n">
         <v>-13.21</v>
       </c>
       <c r="H26" t="n">
-        <v>9.021226749399331</v>
+        <v>4.563412132168279</v>
       </c>
       <c r="I26" t="n">
-        <v>0.6601422506785201</v>
+        <v>0.3339347562573811</v>
       </c>
       <c r="J26" t="n">
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.9275703628046963</v>
+        <v>0.4692139957726764</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2370,11 +2370,11 @@
       </c>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="n">
-        <v>9.021226749399331</v>
+        <v>4.563412132168279</v>
       </c>
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="n">
-        <v>0.6601422506785201</v>
+        <v>0.3339347562573811</v>
       </c>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="inlineStr"/>
@@ -2403,10 +2403,10 @@
         <v>270.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1013955796569955</v>
+        <v>0.1013955793602133</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2406785854081312</v>
+        <v>0.2406785847036712</v>
       </c>
       <c r="G27" t="n">
         <v>-0.332925</v>
@@ -2478,25 +2478,25 @@
         <v>104.15</v>
       </c>
       <c r="E28" t="n">
-        <v>6.766253893937488</v>
+        <v>6.766253892867832</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2961120057517942</v>
+        <v>0.2961120057049828</v>
       </c>
       <c r="G28" t="n">
         <v>-13.21</v>
       </c>
       <c r="H28" t="n">
-        <v>6.182032002992508</v>
+        <v>2.989832425770465</v>
       </c>
       <c r="I28" t="n">
-        <v>0.2705446654415486</v>
+        <v>0.1308442293674332</v>
       </c>
       <c r="J28" t="n">
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.9136565224860334</v>
+        <v>0.4418741113043342</v>
       </c>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
@@ -2516,11 +2516,11 @@
       </c>
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="n">
-        <v>6.182032002992508</v>
+        <v>2.989832425770465</v>
       </c>
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="n">
-        <v>0.2705446654415486</v>
+        <v>0.1308442293674332</v>
       </c>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="inlineStr"/>
@@ -2549,25 +2549,25 @@
         <v>824.3</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1308423264807957</v>
+        <v>0.1308423263315017</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2719810760859471</v>
+        <v>0.2719810757756105</v>
       </c>
       <c r="G29" t="n">
         <v>-2.20113372715757</v>
       </c>
       <c r="H29" t="n">
-        <v>0.125037675289547</v>
+        <v>0.059079127950144</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2599149861610547</v>
+        <v>0.122807391356328</v>
       </c>
       <c r="J29" t="n">
         <v>-2.201133727157571</v>
       </c>
       <c r="K29" t="n">
-        <v>0.9556362887501794</v>
+        <v>0.4515291771904247</v>
       </c>
       <c r="L29" t="n">
         <v>0.129384</v>
@@ -2603,11 +2603,11 @@
       </c>
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="n">
-        <v>0.125037675289547</v>
+        <v>0.059079127950144</v>
       </c>
       <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="n">
-        <v>0.2599149861610547</v>
+        <v>0.122807391356328</v>
       </c>
       <c r="AB29" t="inlineStr"/>
       <c r="AC29" t="n">
@@ -2644,10 +2644,10 @@
         <v>126.11004</v>
       </c>
       <c r="E30" t="n">
-        <v>0.007105612026366954</v>
+        <v>0.007105612027473721</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06718413989473716</v>
+        <v>0.06718413990520174</v>
       </c>
       <c r="G30" t="n">
         <v>-0.078476895921783</v>

</xml_diff>

<commit_message>
from roar; yield rerun
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP/compiled_results.xlsx
+++ b/application/output_max_withoutMP/compiled_results.xlsx
@@ -616,25 +616,25 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.81382214929636</v>
+        <v>17.81382211868636</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5695516939990893</v>
+        <v>0.5695516930204122</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
       </c>
       <c r="H2" t="n">
-        <v>10.33377596184603</v>
+        <v>10.33377596184747</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3303962257593862</v>
+        <v>0.3303962257594323</v>
       </c>
       <c r="J2" t="n">
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5800987500177894</v>
+        <v>0.5800987510146708</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -654,11 +654,11 @@
       </c>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="n">
-        <v>10.33377596184603</v>
+        <v>10.33377596184747</v>
       </c>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
-        <v>0.3303962257593862</v>
+        <v>0.3303962257594323</v>
       </c>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
@@ -687,27 +687,29 @@
         <v>122.16</v>
       </c>
       <c r="E3" t="n">
-        <v>6.94137006466926</v>
+        <v>2.555301938109797</v>
       </c>
       <c r="F3" t="n">
-        <v>0.356305621468374</v>
+        <v>0.3122195099690078</v>
       </c>
       <c r="G3" t="n">
-        <v>-13.21</v>
+        <v>-5.549610203628807</v>
       </c>
       <c r="H3" t="n">
-        <v>3.765885265022366</v>
+        <v>3.765850237785174</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1933056554010884</v>
+        <v>0.1933038574272878</v>
       </c>
       <c r="J3" t="n">
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5425276609570595</v>
-      </c>
-      <c r="L3" t="inlineStr"/>
+        <v>0.6191280533573189</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.08</v>
+      </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
@@ -725,11 +727,11 @@
       </c>
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="n">
-        <v>3.765885265022366</v>
+        <v>3.765850237785174</v>
       </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="n">
-        <v>0.1933056554010884</v>
+        <v>0.1933038574272878</v>
       </c>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
@@ -758,27 +760,29 @@
         <v>90.08</v>
       </c>
       <c r="E4" t="n">
-        <v>20.06614449001378</v>
+        <v>7.37994235935547</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7595227107574315</v>
+        <v>0.665423610156116</v>
       </c>
       <c r="G4" t="n">
-        <v>-13.21</v>
+        <v>-5.545419566893607</v>
       </c>
       <c r="H4" t="n">
-        <v>4.789907146774331</v>
+        <v>4.789896768113398</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1813025547685536</v>
+        <v>0.1813021619263368</v>
       </c>
       <c r="J4" t="n">
         <v>-13.21</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2387059033267751</v>
-      </c>
-      <c r="L4" t="inlineStr"/>
+        <v>0.2724612700228674</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.13</v>
+      </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
@@ -796,11 +800,11 @@
       </c>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="n">
-        <v>4.789907146774331</v>
+        <v>4.789896768113398</v>
       </c>
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="n">
-        <v>0.1813025547685536</v>
+        <v>0.1813021619263368</v>
       </c>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr"/>
@@ -829,27 +833,29 @@
         <v>90.08</v>
       </c>
       <c r="E5" t="n">
-        <v>22.34089253733244</v>
+        <v>8.294245459149197</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8456240943116801</v>
+        <v>0.7479521117530136</v>
       </c>
       <c r="G5" t="n">
-        <v>-13.21</v>
+        <v>-5.544759808667547</v>
       </c>
       <c r="H5" t="n">
-        <v>8.273785303551145</v>
+        <v>8.273785303549536</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3131706663980993</v>
+        <v>0.3131706663980384</v>
       </c>
       <c r="J5" t="n">
         <v>-13.21</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3703426481160208</v>
-      </c>
-      <c r="L5" t="inlineStr"/>
+        <v>0.418704167655927</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.14</v>
+      </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
@@ -867,11 +873,11 @@
       </c>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="n">
-        <v>8.273785303551145</v>
+        <v>8.273785303549536</v>
       </c>
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="n">
-        <v>0.3131706663980993</v>
+        <v>0.3131706663980384</v>
       </c>
       <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="inlineStr"/>
@@ -900,27 +906,29 @@
         <v>90.08</v>
       </c>
       <c r="E6" t="n">
-        <v>20.06614449001378</v>
+        <v>7.37994235935547</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7595227107574315</v>
+        <v>0.665423610156116</v>
       </c>
       <c r="G6" t="n">
-        <v>-13.21</v>
+        <v>-5.545419566893607</v>
       </c>
       <c r="H6" t="n">
-        <v>4.789907146774331</v>
+        <v>4.789896768113398</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1813025547685536</v>
+        <v>0.1813021619263368</v>
       </c>
       <c r="J6" t="n">
         <v>-13.21</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2387059033267751</v>
-      </c>
-      <c r="L6" t="inlineStr"/>
+        <v>0.2724612700228674</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.13</v>
+      </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
@@ -938,11 +946,11 @@
       </c>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="n">
-        <v>4.789907146774331</v>
+        <v>4.789896768113398</v>
       </c>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="n">
-        <v>0.1813025547685536</v>
+        <v>0.1813021619263368</v>
       </c>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="inlineStr"/>
@@ -971,27 +979,29 @@
         <v>90.08</v>
       </c>
       <c r="E7" t="n">
-        <v>22.34089253733244</v>
+        <v>8.294245459149197</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8456240943116801</v>
+        <v>0.7479521117530136</v>
       </c>
       <c r="G7" t="n">
-        <v>-13.21</v>
+        <v>-5.544759808667547</v>
       </c>
       <c r="H7" t="n">
-        <v>8.273785303551145</v>
+        <v>8.273785303549536</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3131706663980993</v>
+        <v>0.3131706663980384</v>
       </c>
       <c r="J7" t="n">
         <v>-13.21</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3703426481160208</v>
-      </c>
-      <c r="L7" t="inlineStr"/>
+        <v>0.418704167655927</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.14</v>
+      </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -1009,11 +1019,11 @@
       </c>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="n">
-        <v>8.273785303551145</v>
+        <v>8.273785303549536</v>
       </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="n">
-        <v>0.3131706663980993</v>
+        <v>0.3131706663980384</v>
       </c>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
@@ -1042,27 +1052,29 @@
         <v>137.11</v>
       </c>
       <c r="E8" t="n">
-        <v>9.055951945825333</v>
+        <v>3.354728528907292</v>
       </c>
       <c r="F8" t="n">
-        <v>0.521737066370266</v>
+        <v>0.4600748684385398</v>
       </c>
       <c r="G8" t="n">
-        <v>-13.21</v>
+        <v>-5.549441423005486</v>
       </c>
       <c r="H8" t="n">
-        <v>3.201830994039559</v>
+        <v>3.201847249820655</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1844658540412944</v>
+        <v>0.1844667905793405</v>
       </c>
       <c r="J8" t="n">
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>0.3535609523099952</v>
-      </c>
-      <c r="L8" t="inlineStr"/>
+        <v>0.4009495045999952</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.07000000000000001</v>
+      </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
@@ -1080,11 +1092,11 @@
       </c>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="n">
-        <v>3.201830994039559</v>
+        <v>3.201847249820655</v>
       </c>
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="n">
-        <v>0.1844658540412944</v>
+        <v>0.1844667905793405</v>
       </c>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
@@ -1113,25 +1125,25 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.844697657836357</v>
+        <v>2.844697655376507</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2800995811875959</v>
+        <v>0.2800995809453898</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
       </c>
       <c r="H9" t="n">
-        <v>1.268691931624992</v>
+        <v>1.26871546942082</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1249201572354529</v>
+        <v>0.1249224748549494</v>
       </c>
       <c r="J9" t="n">
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.445984805495971</v>
+        <v>0.445993080151395</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1151,11 +1163,11 @@
       </c>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="n">
-        <v>1.268691931624992</v>
+        <v>1.26871546942082</v>
       </c>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
-        <v>0.1249201572354529</v>
+        <v>0.1249224748549494</v>
       </c>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="inlineStr"/>
@@ -1184,27 +1196,29 @@
         <v>90.12</v>
       </c>
       <c r="E10" t="n">
-        <v>12.89443785011522</v>
+        <v>5.008732116108107</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4882834990112545</v>
+        <v>0.4516357717891071</v>
       </c>
       <c r="G10" t="n">
-        <v>-13.21</v>
+        <v>-5.547686668594033</v>
       </c>
       <c r="H10" t="n">
-        <v>12.86101832859688</v>
+        <v>12.86101832859704</v>
       </c>
       <c r="I10" t="n">
-        <v>0.48701797653622</v>
+        <v>0.4870179765362261</v>
       </c>
       <c r="J10" t="n">
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>0.9974082219087946</v>
-      </c>
-      <c r="L10" t="inlineStr"/>
+        <v>1.078342343448474</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.11</v>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -1222,11 +1236,11 @@
       </c>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="n">
-        <v>12.86101832859688</v>
+        <v>12.86101832859704</v>
       </c>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
-        <v>0.48701797653622</v>
+        <v>0.4870179765362261</v>
       </c>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="inlineStr"/>
@@ -1255,27 +1269,29 @@
         <v>74.12</v>
       </c>
       <c r="E11" t="n">
-        <v>11.19787297467806</v>
+        <v>4.161856555785656</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3487541619380868</v>
+        <v>0.3085281699142969</v>
       </c>
       <c r="G11" t="n">
-        <v>-13.21</v>
+        <v>-5.549820853803196</v>
       </c>
       <c r="H11" t="n">
-        <v>8.787635674310453</v>
+        <v>8.7876356743113</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2736880943319939</v>
+        <v>0.2736880943320203</v>
       </c>
       <c r="J11" t="n">
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7847593640490544</v>
-      </c>
-      <c r="L11" t="inlineStr"/>
+        <v>0.8870765168964814</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.04</v>
+      </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
@@ -1293,11 +1309,11 @@
       </c>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="n">
-        <v>8.787635674310453</v>
+        <v>8.7876356743113</v>
       </c>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
-        <v>0.2736880943319939</v>
+        <v>0.2736880943320203</v>
       </c>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="inlineStr"/>
@@ -1326,25 +1342,25 @@
         <v>146.1</v>
       </c>
       <c r="E12" t="n">
-        <v>12.48937108880217</v>
+        <v>12.48937108880216</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7667243171293756</v>
+        <v>0.7667243171293748</v>
       </c>
       <c r="G12" t="n">
         <v>-13.21</v>
       </c>
       <c r="H12" t="n">
-        <v>4.983742289914067</v>
+        <v>4.983742289914098</v>
       </c>
       <c r="I12" t="n">
-        <v>0.3059526678176101</v>
+        <v>0.305952667817612</v>
       </c>
       <c r="J12" t="n">
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>0.3990386909379636</v>
+        <v>0.3990386909379665</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1364,11 +1380,11 @@
       </c>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="n">
-        <v>4.983742289914067</v>
+        <v>4.983742289914098</v>
       </c>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
-        <v>0.3059526678176101</v>
+        <v>0.305952667817612</v>
       </c>
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="inlineStr"/>
@@ -1397,27 +1413,29 @@
         <v>163.15</v>
       </c>
       <c r="E13" t="n">
-        <v>7.096204240677997</v>
+        <v>2.611823931690337</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4864762432011422</v>
+        <v>0.4262860820839183</v>
       </c>
       <c r="G13" t="n">
-        <v>-13.21</v>
+        <v>-5.548570274707735</v>
       </c>
       <c r="H13" t="n">
-        <v>3.08763752503665</v>
+        <v>3.087637525036674</v>
       </c>
       <c r="I13" t="n">
-        <v>0.211671233324478</v>
+        <v>0.2116712333244796</v>
       </c>
       <c r="J13" t="n">
         <v>-13.21</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4351111411558873</v>
-      </c>
-      <c r="L13" t="inlineStr"/>
+        <v>0.4965473709338937</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.15</v>
+      </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -1435,11 +1453,11 @@
       </c>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="n">
-        <v>3.08763752503665</v>
+        <v>3.087637525036674</v>
       </c>
       <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="n">
-        <v>0.211671233324478</v>
+        <v>0.2116712333244796</v>
       </c>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="inlineStr"/>
@@ -1468,27 +1486,29 @@
         <v>256.4</v>
       </c>
       <c r="E14" t="n">
-        <v>2.761960143974937</v>
+        <v>1.016994536421393</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2975663924620421</v>
+        <v>0.2607839207207009</v>
       </c>
       <c r="G14" t="n">
-        <v>-13.21</v>
+        <v>-5.550180402242267</v>
       </c>
       <c r="H14" t="n">
-        <v>0.716460988511289</v>
+        <v>0.716460988511275</v>
       </c>
       <c r="I14" t="n">
-        <v>0.07718964089911483</v>
+        <v>0.07718964089911332</v>
       </c>
       <c r="J14" t="n">
         <v>-13.21</v>
       </c>
       <c r="K14" t="n">
-        <v>0.259403087359609</v>
-      </c>
-      <c r="L14" t="inlineStr"/>
+        <v>0.2959907983812517</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.1</v>
+      </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
@@ -1506,11 +1526,11 @@
       </c>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="n">
-        <v>0.716460988511289</v>
+        <v>0.716460988511275</v>
       </c>
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="n">
-        <v>0.07718964089911483</v>
+        <v>0.07718964089911332</v>
       </c>
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="inlineStr"/>
@@ -1539,27 +1559,29 @@
         <v>242.44</v>
       </c>
       <c r="E15" t="n">
-        <v>2.677177422360339</v>
+        <v>0.9874314723701774</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2727280961920816</v>
+        <v>0.2393940680876117</v>
       </c>
       <c r="G15" t="n">
-        <v>-13.21</v>
+        <v>-5.550717505065815</v>
       </c>
       <c r="H15" t="n">
-        <v>0.7283461481432379</v>
+        <v>0.72835282365734</v>
       </c>
       <c r="I15" t="n">
-        <v>0.07419771909506445</v>
+        <v>0.07419839913974022</v>
       </c>
       <c r="J15" t="n">
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.2720574819061077</v>
-      </c>
-      <c r="L15" t="inlineStr"/>
+        <v>0.3099425133315568</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.005</v>
+      </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
@@ -1577,11 +1599,11 @@
       </c>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="n">
-        <v>0.7283461481432379</v>
+        <v>0.72835282365734</v>
       </c>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="n">
-        <v>0.07419771909506445</v>
+        <v>0.07419839913974022</v>
       </c>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
@@ -1610,27 +1632,29 @@
         <v>74.12</v>
       </c>
       <c r="E16" t="n">
-        <v>12.52385380260009</v>
+        <v>4.68640372837228</v>
       </c>
       <c r="F16" t="n">
-        <v>0.39005140949873</v>
+        <v>0.3474539429141642</v>
       </c>
       <c r="G16" t="n">
-        <v>-13.21</v>
+        <v>-5.549184128068436</v>
       </c>
       <c r="H16" t="n">
-        <v>12.3642424889837</v>
+        <v>12.36424248898358</v>
       </c>
       <c r="I16" t="n">
-        <v>0.385080366333479</v>
+        <v>0.3850803663334754</v>
       </c>
       <c r="J16" t="n">
         <v>-13.21</v>
       </c>
       <c r="K16" t="n">
-        <v>0.9872554154550053</v>
-      </c>
-      <c r="L16" t="inlineStr"/>
+        <v>1.108291830289019</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.06</v>
+      </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
@@ -1648,11 +1672,11 @@
       </c>
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="n">
-        <v>12.3642424889837</v>
+        <v>12.36424248898358</v>
       </c>
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="n">
-        <v>0.385080366333479</v>
+        <v>0.3850803663334754</v>
       </c>
       <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="inlineStr"/>
@@ -1681,27 +1705,29 @@
         <v>89.06999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>24.24659125876742</v>
+        <v>8.860211623681527</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9074664869966653</v>
+        <v>0.7940334091095929</v>
       </c>
       <c r="G17" t="n">
-        <v>-13.21</v>
+        <v>-5.516810175512664</v>
       </c>
       <c r="H17" t="n">
-        <v>21.15294223104609</v>
+        <v>21.15294223104569</v>
       </c>
       <c r="I17" t="n">
-        <v>0.7916818480251235</v>
+        <v>0.7916818480251087</v>
       </c>
       <c r="J17" t="n">
         <v>-13.21</v>
       </c>
       <c r="K17" t="n">
-        <v>0.872408909165626</v>
-      </c>
-      <c r="L17" t="inlineStr"/>
+        <v>0.9970384607782169</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.6899999999999999</v>
+      </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
@@ -1719,11 +1745,11 @@
       </c>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="n">
-        <v>21.15294223104609</v>
+        <v>21.15294223104569</v>
       </c>
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="n">
-        <v>0.7916818480251235</v>
+        <v>0.7916818480251087</v>
       </c>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
@@ -1752,27 +1778,29 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>10.42241535083183</v>
+        <v>3.836460769542606</v>
       </c>
       <c r="F18" t="n">
-        <v>0.6135132739858409</v>
+        <v>0.5375941613289151</v>
       </c>
       <c r="G18" t="n">
-        <v>-13.21</v>
+        <v>-5.549254244910696</v>
       </c>
       <c r="H18" t="n">
-        <v>4.807363077610548</v>
+        <v>4.807363077609868</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2829844102066129</v>
+        <v>0.2829844102065729</v>
       </c>
       <c r="J18" t="n">
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>0.4612523024451201</v>
-      </c>
-      <c r="L18" t="inlineStr"/>
+        <v>0.526390408532423</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.07000000000000001</v>
+      </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
@@ -1790,11 +1818,11 @@
       </c>
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="n">
-        <v>4.807363077610548</v>
+        <v>4.807363077609868</v>
       </c>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="n">
-        <v>0.2829844102066129</v>
+        <v>0.2829844102065729</v>
       </c>
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="inlineStr"/>
@@ -1823,25 +1851,25 @@
         <v>272.25</v>
       </c>
       <c r="E19" t="n">
-        <v>3.969093040440947</v>
+        <v>3.969093036182524</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4540541188048531</v>
+        <v>0.4540541183177003</v>
       </c>
       <c r="G19" t="n">
         <v>-13.21</v>
       </c>
       <c r="H19" t="n">
-        <v>1.076926979514537</v>
+        <v>1.076926979514566</v>
       </c>
       <c r="I19" t="n">
-        <v>0.1231976992523011</v>
+        <v>0.1231976992523044</v>
       </c>
       <c r="J19" t="n">
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.2713282275174118</v>
+        <v>0.271328227808526</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1861,11 +1889,11 @@
       </c>
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="n">
-        <v>1.076926979514537</v>
+        <v>1.076926979514566</v>
       </c>
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="n">
-        <v>0.1231976992523011</v>
+        <v>0.1231976992523044</v>
       </c>
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="inlineStr"/>
@@ -1894,10 +1922,10 @@
         <v>268.5</v>
       </c>
       <c r="E20" t="n">
-        <v>0.09996363102997334</v>
+        <v>0.09996363049204143</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2355252488649593</v>
+        <v>0.2355252475975329</v>
       </c>
       <c r="G20" t="n">
         <v>-0.332925</v>
@@ -1906,12 +1934,8 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
-      <c r="L20" t="n">
-        <v>0.0272</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0.028</v>
-      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
           <t>media:reset;c_sources:EX_sucr_e;media:reset;c_sources:EX_sucr_e;EX_sucr_e:(-0.332925,1000);EX_k_e:(-0.1,1000);EX_nh4_e:(-0.09,1000);EX_ca2_e:(-0.002844,1000);EX_mg2_e:(-0.004689,1000);EX_pi_e:(-0.01,1000);EX_no3_e:(-0.003217,1000);EX_cl_e:(-0.00643,1000);EX_so4_e:(-0.002,1000);EX_h_e:(-1000,1000);EX_h2o_e:(-1000,1000);EX_btn_c:(-0.01,1000);EX_o2_e:(-26.25403530509562,1000);EX_co2_e:(0,1000);EX_thm_e:(-1000,1000);EX_ribflv_e:(-1000,1000);EX_nac_e:(-1000,1000);EX_pydxn_e:(-1000,1000);EX_fol_e:(-1000,1000);EX_pnto__R_e:(-1000,1000);EX_4abz_e:(-1000,1000);EX_cu2_e:(-1000,1000);EX_fe2_e:(-1000,1000);EX_fe3_e:(-1000,1000);EX_mn2_e:(-1000,1000);EX_na1_e:(-1000,1000);EX_ni2_e:(-1000,1000);EX_zn2_e:(-1000,1000);EX_cobalt2_e:(-1000,1000);EX_inost_e:(-1000,1000);EX_asp__L_e:(-0.00046,1000);EX_thr__L_e:(-0.000276,1000);EX_ser__L_e:(-0.000334,1000);EX_glu__L_e:(-0.001013,1000);EX_gly_e:(-0.000747,1000);EX_tyr__L_e:(-0.000094,1000);EX_lys__L_e:(-0.000216,1000);EX_arg__L_e:(-0.000236,1000);EX_trp__L_e:(-0.000023,1000);EX_chol_e:(-0.090319,1000);EX_ala__L_e:(-0.001179,1000);EX_val__L_e:(-0.000463,1000);EX_met__L_e:(-0.000132,1000);EX_ile__L_e:(-0.000253,1000);EX_leu__L_e:(-0.000709,1000);EX_phe__L_e:(-0.000229,1000);EX_his__L_e:(-0.000205,1000);EX_pro__L_e:(-0.000761,1000);BIOMASS_AERO_SC_hvd:(0.0133333333333333,1000)</t>
@@ -1973,10 +1997,10 @@
         <v>242.44</v>
       </c>
       <c r="E21" t="n">
-        <v>0.114167372765945</v>
+        <v>0.1141673830273931</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2428831803376595</v>
+        <v>0.2428832021681798</v>
       </c>
       <c r="G21" t="n">
         <v>-0.332925</v>
@@ -1985,12 +2009,8 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
-      <c r="L21" t="n">
-        <v>0.0036</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0.006</v>
-      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
           <t>media:reset;c_sources:EX_sucr_e;media:reset;c_sources:EX_sucr_e;EX_sucr_e:(-0.332925,1000);EX_k_e:(-0.1,1000);EX_nh4_e:(-0.09,1000);EX_ca2_e:(-0.002844,1000);EX_mg2_e:(-0.004689,1000);EX_pi_e:(-0.01,1000);EX_no3_e:(-0.003217,1000);EX_cl_e:(-0.00643,1000);EX_so4_e:(-0.002,1000);EX_h_e:(-1000,1000);EX_h2o_e:(-1000,1000);EX_btn_c:(-0.01,1000);EX_o2_e:(-26.25403530509562,1000);EX_co2_e:(0,1000);EX_thm_e:(-1000,1000);EX_ribflv_e:(-1000,1000);EX_nac_e:(-1000,1000);EX_pydxn_e:(-1000,1000);EX_fol_e:(-1000,1000);EX_pnto__R_e:(-1000,1000);EX_4abz_e:(-1000,1000);EX_cu2_e:(-1000,1000);EX_fe2_e:(-1000,1000);EX_fe3_e:(-1000,1000);EX_mn2_e:(-1000,1000);EX_na1_e:(-1000,1000);EX_ni2_e:(-1000,1000);EX_zn2_e:(-1000,1000);EX_cobalt2_e:(-1000,1000);EX_inost_e:(-1000,1000);EX_asp__L_e:(-0.00046,1000);EX_thr__L_e:(-0.000276,1000);EX_ser__L_e:(-0.000334,1000);EX_glu__L_e:(-0.001013,1000);EX_gly_e:(-0.000747,1000);EX_tyr__L_e:(-0.000094,1000);EX_lys__L_e:(-0.000216,1000);EX_arg__L_e:(-0.000236,1000);EX_trp__L_e:(-0.000023,1000);EX_chol_e:(-0.090319,1000);EX_ala__L_e:(-0.001179,1000);EX_val__L_e:(-0.000463,1000);EX_met__L_e:(-0.000132,1000);EX_ile__L_e:(-0.000253,1000);EX_leu__L_e:(-0.000709,1000);EX_phe__L_e:(-0.000229,1000);EX_his__L_e:(-0.000205,1000);EX_pro__L_e:(-0.000761,1000);BIOMASS_AERO_SC_hvd:(0.0133333333333333,1000)</t>
@@ -2048,27 +2068,29 @@
         <v>103.1</v>
       </c>
       <c r="E22" t="n">
-        <v>12.48937108880214</v>
+        <v>4.826633115573237</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5410628137990309</v>
+        <v>0.497938311736443</v>
       </c>
       <c r="G22" t="n">
-        <v>-13.21</v>
+        <v>-5.547262026771105</v>
       </c>
       <c r="H22" t="n">
-        <v>4.768756988393707</v>
+        <v>4.768759915832433</v>
       </c>
       <c r="I22" t="n">
-        <v>0.2065914333170446</v>
+        <v>0.2065915601391419</v>
       </c>
       <c r="J22" t="n">
         <v>-13.21</v>
       </c>
       <c r="K22" t="n">
-        <v>0.3818252299885087</v>
-      </c>
-      <c r="L22" t="inlineStr"/>
+        <v>0.414893883980733</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.13</v>
+      </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
@@ -2086,11 +2108,11 @@
       </c>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="n">
-        <v>4.768756988393707</v>
+        <v>4.768759915832433</v>
       </c>
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="n">
-        <v>0.2065914333170446</v>
+        <v>0.2065915601391419</v>
       </c>
       <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="inlineStr"/>
@@ -2119,25 +2141,25 @@
         <v>329.4</v>
       </c>
       <c r="E23" t="n">
-        <v>2.511143877685606</v>
+        <v>2.511143874209327</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3475710878604674</v>
+        <v>0.3475710873793104</v>
       </c>
       <c r="G23" t="n">
         <v>-13.21</v>
       </c>
       <c r="H23" t="n">
-        <v>0.491953794688782</v>
+        <v>0.49195678905012</v>
       </c>
       <c r="I23" t="n">
-        <v>0.06809204248171426</v>
+        <v>0.06809245693563581</v>
       </c>
       <c r="J23" t="n">
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1959082468592723</v>
+        <v>0.1959094395596988</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2157,11 +2179,11 @@
       </c>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="n">
-        <v>0.491953794688782</v>
+        <v>0.49195678905012</v>
       </c>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="n">
-        <v>0.06809204248171426</v>
+        <v>0.06809245693563581</v>
       </c>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
@@ -2190,27 +2212,29 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>3.969093040440451</v>
+        <v>1.465955758988992</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3806549571203185</v>
+        <v>0.3345898405304283</v>
       </c>
       <c r="G24" t="n">
-        <v>-13.21</v>
+        <v>-5.550743282537625</v>
       </c>
       <c r="H24" t="n">
-        <v>1.076921922608241</v>
+        <v>1.076926979514542</v>
       </c>
       <c r="I24" t="n">
-        <v>0.1032819498297476</v>
+        <v>0.1032824348111858</v>
       </c>
       <c r="J24" t="n">
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.2713269534464565</v>
-      </c>
-      <c r="L24" t="inlineStr"/>
+        <v>0.3086837145068458</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.0002</v>
+      </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
@@ -2228,11 +2252,11 @@
       </c>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="n">
-        <v>1.076921922608241</v>
+        <v>1.076926979514542</v>
       </c>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="n">
-        <v>0.1032819498297476</v>
+        <v>0.1032824348111858</v>
       </c>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="inlineStr"/>
@@ -2261,27 +2285,29 @@
         <v>246.3</v>
       </c>
       <c r="E25" t="n">
-        <v>2.957467002868275</v>
+        <v>1.116107087963433</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3060784626771426</v>
+        <v>0.2748980962125347</v>
       </c>
       <c r="G25" t="n">
-        <v>-13.21</v>
+        <v>-5.550726324289703</v>
       </c>
       <c r="H25" t="n">
-        <v>1.323884235524466</v>
+        <v>1.323884560568239</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1370133466168315</v>
+        <v>0.1370133802567328</v>
       </c>
       <c r="J25" t="n">
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.4476412532212557</v>
-      </c>
-      <c r="L25" t="inlineStr"/>
+        <v>0.4984151659995575</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.003</v>
+      </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
@@ -2299,11 +2325,11 @@
       </c>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="n">
-        <v>1.323884235524466</v>
+        <v>1.323884560568239</v>
       </c>
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="n">
-        <v>0.1370133466168315</v>
+        <v>0.1370133802567328</v>
       </c>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="inlineStr"/>
@@ -2332,25 +2358,25 @@
         <v>174.15</v>
       </c>
       <c r="E26" t="n">
-        <v>9.725652204072677</v>
+        <v>9.725652187360838</v>
       </c>
       <c r="F26" t="n">
-        <v>0.7116896752141317</v>
+        <v>0.7116896739912171</v>
       </c>
       <c r="G26" t="n">
         <v>-13.21</v>
       </c>
       <c r="H26" t="n">
-        <v>4.563412132168279</v>
+        <v>4.563412132168618</v>
       </c>
       <c r="I26" t="n">
-        <v>0.3339347562573811</v>
+        <v>0.3339347562574059</v>
       </c>
       <c r="J26" t="n">
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.4692139957726764</v>
+        <v>0.4692139965789738</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2370,11 +2396,11 @@
       </c>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="n">
-        <v>4.563412132168279</v>
+        <v>4.563412132168618</v>
       </c>
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="n">
-        <v>0.3339347562573811</v>
+        <v>0.3339347562574059</v>
       </c>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="inlineStr"/>
@@ -2403,10 +2429,10 @@
         <v>270.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1013955793602133</v>
+        <v>0.1013955788142332</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2406785847036712</v>
+        <v>0.2406785834077004</v>
       </c>
       <c r="G27" t="n">
         <v>-0.332925</v>
@@ -2415,12 +2441,8 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
-      <c r="L27" t="n">
-        <v>0.006</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0.0092</v>
-      </c>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr">
         <is>
           <t>media:reset;c_sources:EX_sucr_e;media:reset;c_sources:EX_sucr_e;EX_sucr_e:(-0.332925,1000);EX_k_e:(-0.1,1000);EX_nh4_e:(-0.09,1000);EX_ca2_e:(-0.002844,1000);EX_mg2_e:(-0.004689,1000);EX_pi_e:(-0.01,1000);EX_no3_e:(-0.003217,1000);EX_cl_e:(-0.00643,1000);EX_so4_e:(-0.002,1000);EX_h_e:(-1000,1000);EX_h2o_e:(-1000,1000);EX_btn_c:(-0.01,1000);EX_o2_e:(-26.25403530509562,1000);EX_co2_e:(0,1000);EX_thm_e:(-1000,1000);EX_ribflv_e:(-1000,1000);EX_nac_e:(-1000,1000);EX_pydxn_e:(-1000,1000);EX_fol_e:(-1000,1000);EX_pnto__R_e:(-1000,1000);EX_4abz_e:(-1000,1000);EX_cu2_e:(-1000,1000);EX_fe2_e:(-1000,1000);EX_fe3_e:(-1000,1000);EX_mn2_e:(-1000,1000);EX_na1_e:(-1000,1000);EX_ni2_e:(-1000,1000);EX_zn2_e:(-1000,1000);EX_cobalt2_e:(-1000,1000);EX_inost_e:(-1000,1000);EX_asp__L_e:(-0.00046,1000);EX_thr__L_e:(-0.000276,1000);EX_ser__L_e:(-0.000334,1000);EX_glu__L_e:(-0.001013,1000);EX_gly_e:(-0.000747,1000);EX_tyr__L_e:(-0.000094,1000);EX_lys__L_e:(-0.000216,1000);EX_arg__L_e:(-0.000236,1000);EX_trp__L_e:(-0.000023,1000);EX_chol_e:(-0.090319,1000);EX_ala__L_e:(-0.001179,1000);EX_val__L_e:(-0.000463,1000);EX_met__L_e:(-0.000132,1000);EX_ile__L_e:(-0.000253,1000);EX_leu__L_e:(-0.000709,1000);EX_phe__L_e:(-0.000229,1000);EX_his__L_e:(-0.000205,1000);EX_pro__L_e:(-0.000761,1000);BIOMASS_AERO_SC_hvd:(0.0133333333333333,1000)</t>
@@ -2478,27 +2500,29 @@
         <v>104.15</v>
       </c>
       <c r="E28" t="n">
-        <v>6.766253892867832</v>
+        <v>2.491549780251542</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2961120057049828</v>
+        <v>0.2594955561592948</v>
       </c>
       <c r="G28" t="n">
-        <v>-13.21</v>
+        <v>-5.55073108000964</v>
       </c>
       <c r="H28" t="n">
-        <v>2.989832425770465</v>
+        <v>2.989848416694203</v>
       </c>
       <c r="I28" t="n">
-        <v>0.1308442293674332</v>
+        <v>0.1308449291792606</v>
       </c>
       <c r="J28" t="n">
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.4418741113043342</v>
-      </c>
-      <c r="L28" t="inlineStr"/>
+        <v>0.5042280149835772</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.001</v>
+      </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
@@ -2516,11 +2540,11 @@
       </c>
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="n">
-        <v>2.989832425770465</v>
+        <v>2.989848416694203</v>
       </c>
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="n">
-        <v>0.1308442293674332</v>
+        <v>0.1308449291792606</v>
       </c>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="inlineStr"/>
@@ -2549,32 +2573,30 @@
         <v>824.3</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1308423263315017</v>
+        <v>0.1308423337395128</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2719810757756105</v>
+        <v>0.2719810911745942</v>
       </c>
       <c r="G29" t="n">
         <v>-2.20113372715757</v>
       </c>
       <c r="H29" t="n">
-        <v>0.059079127950144</v>
+        <v>0.059078934933109</v>
       </c>
       <c r="I29" t="n">
-        <v>0.122807391356328</v>
+        <v>0.1228069901330977</v>
       </c>
       <c r="J29" t="n">
         <v>-2.201133727157571</v>
       </c>
       <c r="K29" t="n">
-        <v>0.4515291771904247</v>
+        <v>0.451527676437858</v>
       </c>
       <c r="L29" t="n">
-        <v>0.129384</v>
-      </c>
-      <c r="M29" t="n">
-        <v>0.1468</v>
-      </c>
+        <v>0.14</v>
+      </c>
+      <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr">
         <is>
           <t>c_sources:EX_glc__D_e;BIOMASS_AERO_SC_hvd:(0.009615384615,0.14);EX_glc__D_e:(-2.20113372715757,1000);EX_nh4_e:(-0.181824845165991,1000);EX_o2_e:(-26.25403530509562,1000)</t>
@@ -2603,11 +2625,11 @@
       </c>
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="n">
-        <v>0.059079127950144</v>
+        <v>0.059078934933109</v>
       </c>
       <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="n">
-        <v>0.122807391356328</v>
+        <v>0.1228069901330977</v>
       </c>
       <c r="AB29" t="inlineStr"/>
       <c r="AC29" t="n">
@@ -2644,10 +2666,10 @@
         <v>126.11004</v>
       </c>
       <c r="E30" t="n">
-        <v>0.007105612027473721</v>
+        <v>0.007105612999394498</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06718413990520174</v>
+        <v>0.06718414909479177</v>
       </c>
       <c r="G30" t="n">
         <v>-0.078476895921783</v>
@@ -2656,12 +2678,8 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
-      <c r="L30" t="n">
-        <v>0.1145097305125967</v>
-      </c>
-      <c r="M30" t="n">
-        <v>0.1208420658404822</v>
-      </c>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr">
         <is>
           <t>c_sources:EX_xyl__D_e,EX_glc__D_e;EX_xyl__D_e:(-0.0266525306904169,-0.0266525306904169);EX_glc__D_e:(-0.0518243652313661,-0.0518243652313661);BIOMASS_AERO_SC_hvd:(0,0.0138888888888889);BiomassKim_e:(0,0);EX_btn_c:(0,0.02);ATPM_c:(0,1000);EX_4abz_e:(-1000,1000);EX_fe3_e:(-1000,1000);EX_fol_e:(-1000,1000);EX_inost_e:(-1000,1000);EX_nac_e:(-1000,1000);EX_pnto__R_e:(-1000,1000);EX_pydxn_e:(-1000,1000);EX_ribflv_e:(-1000,1000);EX_thm_e:(-1000,1000);EX_o2_e:(-26.25403530509562,1000)</t>

</xml_diff>

<commit_message>
removed minYield since it was causing issues; reran
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP/compiled_results.xlsx
+++ b/application/output_max_withoutMP/compiled_results.xlsx
@@ -616,10 +616,10 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.81382266698288</v>
+        <v>17.81382210473816</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5695517105508002</v>
+        <v>0.5695516925744543</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
@@ -634,7 +634,7 @@
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5800987331596378</v>
+        <v>0.5800987514688722</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -687,13 +687,13 @@
         <v>122.16</v>
       </c>
       <c r="E3" t="n">
-        <v>2.555302146413386</v>
+        <v>6.941370044788568</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3122195354257759</v>
+        <v>0.3563056204478834</v>
       </c>
       <c r="G3" t="n">
-        <v>-5.549610203536402</v>
+        <v>-13.21</v>
       </c>
       <c r="H3" t="n">
         <v>3.765885265022023</v>
@@ -705,7 +705,7 @@
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.6191337615612632</v>
+        <v>0.5425276625108567</v>
       </c>
       <c r="L3" t="n">
         <v>0.08</v>
@@ -760,13 +760,13 @@
         <v>90.08</v>
       </c>
       <c r="E4" t="n">
-        <v>7.379942970720204</v>
+        <v>20.06614443981965</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6654236653336743</v>
+        <v>0.7595227088575357</v>
       </c>
       <c r="G4" t="n">
-        <v>-5.545419566452449</v>
+        <v>-13.21</v>
       </c>
       <c r="H4" t="n">
         <v>4.789907146773598</v>
@@ -778,7 +778,7 @@
         <v>-13.21</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2724618377941404</v>
+        <v>0.2387059039238457</v>
       </c>
       <c r="L4" t="n">
         <v>0.13</v>
@@ -833,13 +833,13 @@
         <v>90.08</v>
       </c>
       <c r="E5" t="n">
-        <v>8.294246188234464</v>
+        <v>22.34089249430825</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7479521775708778</v>
+        <v>0.8456240926831734</v>
       </c>
       <c r="G5" t="n">
-        <v>-5.544759808141415</v>
+        <v>-13.21</v>
       </c>
       <c r="H5" t="n">
         <v>8.273785303549822</v>
@@ -851,7 +851,7 @@
         <v>-13.21</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4187041308110536</v>
+        <v>0.3703426488291691</v>
       </c>
       <c r="L5" t="n">
         <v>0.14</v>
@@ -906,13 +906,13 @@
         <v>90.08</v>
       </c>
       <c r="E6" t="n">
-        <v>7.379942970720204</v>
+        <v>20.06614443981965</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6654236653336743</v>
+        <v>0.7595227088575357</v>
       </c>
       <c r="G6" t="n">
-        <v>-5.545419566452449</v>
+        <v>-13.21</v>
       </c>
       <c r="H6" t="n">
         <v>4.789907146773598</v>
@@ -924,7 +924,7 @@
         <v>-13.21</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2724618377941404</v>
+        <v>0.2387059039238457</v>
       </c>
       <c r="L6" t="n">
         <v>0.13</v>
@@ -979,13 +979,13 @@
         <v>90.08</v>
       </c>
       <c r="E7" t="n">
-        <v>8.294246188234464</v>
+        <v>22.34089249430825</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7479521775708778</v>
+        <v>0.8456240926831734</v>
       </c>
       <c r="G7" t="n">
-        <v>-5.544759808141415</v>
+        <v>-13.21</v>
       </c>
       <c r="H7" t="n">
         <v>8.273785303549822</v>
@@ -997,7 +997,7 @@
         <v>-13.21</v>
       </c>
       <c r="K7" t="n">
-        <v>0.4187041308110536</v>
+        <v>0.3703426488291691</v>
       </c>
       <c r="L7" t="n">
         <v>0.14</v>
@@ -1052,13 +1052,13 @@
         <v>137.11</v>
       </c>
       <c r="E8" t="n">
-        <v>3.3547287891794</v>
+        <v>9.055951924829568</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4600749041412152</v>
+        <v>0.521737065160645</v>
       </c>
       <c r="G8" t="n">
-        <v>-5.549441422904351</v>
+        <v>-13.21</v>
       </c>
       <c r="H8" t="n">
         <v>3.201832471428046</v>
@@ -1070,7 +1070,7 @@
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>0.4009476228698785</v>
+        <v>0.3535611162697625</v>
       </c>
       <c r="L8" t="n">
         <v>0.07000000000000001</v>
@@ -1125,10 +1125,10 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.844697751491924</v>
+        <v>2.844697670245594</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2800995904092736</v>
+        <v>0.2800995824094558</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
@@ -1143,7 +1143,7 @@
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4459930650824754</v>
+        <v>0.4459930778203139</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1196,13 +1196,13 @@
         <v>90.12</v>
       </c>
       <c r="E10" t="n">
-        <v>5.008732560944163</v>
+        <v>12.8944378446668</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4516358119219428</v>
+        <v>0.488283498804935</v>
       </c>
       <c r="G10" t="n">
-        <v>-5.547686668322433</v>
+        <v>-13.21</v>
       </c>
       <c r="H10" t="n">
         <v>12.86101832859704</v>
@@ -1214,7 +1214,7 @@
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>1.078342247625834</v>
+        <v>0.9974082223302524</v>
       </c>
       <c r="L10" t="n">
         <v>0.11</v>
@@ -1269,13 +1269,13 @@
         <v>74.12</v>
       </c>
       <c r="E11" t="n">
-        <v>4.161856922388838</v>
+        <v>11.19787294998664</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3085281970959751</v>
+        <v>0.3487541611690804</v>
       </c>
       <c r="G11" t="n">
-        <v>-5.549820853721783</v>
+        <v>-13.21</v>
       </c>
       <c r="H11" t="n">
         <v>8.787635674310746</v>
@@ -1287,7 +1287,7 @@
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>0.8870764387439954</v>
+        <v>0.7847593657794829</v>
       </c>
       <c r="L11" t="n">
         <v>0.04</v>
@@ -1342,10 +1342,10 @@
         <v>146.1</v>
       </c>
       <c r="E12" t="n">
-        <v>12.48937108880217</v>
+        <v>12.48937108880209</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7667243171293754</v>
+        <v>0.7667243171293706</v>
       </c>
       <c r="G12" t="n">
         <v>-13.21</v>
@@ -1360,7 +1360,7 @@
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>0.3990386909380138</v>
+        <v>0.3990386909380163</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1413,13 +1413,13 @@
         <v>163.15</v>
       </c>
       <c r="E13" t="n">
-        <v>2.611824148030394</v>
+        <v>7.096204221127857</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4262861174074705</v>
+        <v>0.4864762418608935</v>
       </c>
       <c r="G13" t="n">
-        <v>-5.548570274527612</v>
+        <v>-13.21</v>
       </c>
       <c r="H13" t="n">
         <v>3.087637525036586</v>
@@ -1431,7 +1431,7 @@
         <v>-13.21</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4965473297882351</v>
+        <v>0.4351111423546155</v>
       </c>
       <c r="L13" t="n">
         <v>0.15</v>
@@ -1486,13 +1486,13 @@
         <v>256.4</v>
       </c>
       <c r="E14" t="n">
-        <v>1.016994620429751</v>
+        <v>2.761960154328127</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2607839422648261</v>
+        <v>0.2975663935774678</v>
       </c>
       <c r="G14" t="n">
-        <v>-5.550180402195631</v>
+        <v>-13.21</v>
       </c>
       <c r="H14" t="n">
         <v>0.716460988511337</v>
@@ -1504,7 +1504,7 @@
         <v>-13.21</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2959907739286106</v>
+        <v>0.2594030863872557</v>
       </c>
       <c r="L14" t="n">
         <v>0.1</v>
@@ -1559,13 +1559,13 @@
         <v>242.44</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9874315537026207</v>
+        <v>2.677177417204605</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2393940878060441</v>
+        <v>0.2727280956668592</v>
       </c>
       <c r="G15" t="n">
-        <v>-5.550717505063556</v>
+        <v>-13.21</v>
       </c>
       <c r="H15" t="n">
         <v>0.728351265847033</v>
@@ -1577,7 +1577,7 @@
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.3099418248932406</v>
+        <v>0.2720593940343134</v>
       </c>
       <c r="L15" t="n">
         <v>0.005</v>
@@ -1632,13 +1632,13 @@
         <v>74.12</v>
       </c>
       <c r="E16" t="n">
-        <v>4.686404129847706</v>
+        <v>12.5238538026001</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3474539726882644</v>
+        <v>0.3900514094987304</v>
       </c>
       <c r="G16" t="n">
-        <v>-5.549184127934729</v>
+        <v>-13.21</v>
       </c>
       <c r="H16" t="n">
         <v>12.36424248898357</v>
@@ -1650,7 +1650,7 @@
         <v>-13.21</v>
       </c>
       <c r="K16" t="n">
-        <v>1.108291735317037</v>
+        <v>0.9872554154549937</v>
       </c>
       <c r="L16" t="n">
         <v>0.06</v>
@@ -1705,13 +1705,13 @@
         <v>89.06999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>8.860212302540704</v>
+        <v>24.24659146894868</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7940334703217333</v>
+        <v>0.9074664948630266</v>
       </c>
       <c r="G17" t="n">
-        <v>-5.516810172912661</v>
+        <v>-13.21</v>
       </c>
       <c r="H17" t="n">
         <v>21.15294223104726</v>
@@ -1723,7 +1723,7 @@
         <v>-13.21</v>
       </c>
       <c r="K17" t="n">
-        <v>0.99703838391647</v>
+        <v>0.8724089016032093</v>
       </c>
       <c r="L17" t="n">
         <v>0.6899999999999999</v>
@@ -1778,13 +1778,13 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>3.83646087776361</v>
+        <v>10.42241532098108</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5375941764977421</v>
+        <v>0.6135132722286827</v>
       </c>
       <c r="G18" t="n">
-        <v>-5.549254244868644</v>
+        <v>-13.21</v>
       </c>
       <c r="H18" t="n">
         <v>4.807363077610059</v>
@@ -1796,7 +1796,7 @@
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>0.5263903936797439</v>
+        <v>0.4612523037661422</v>
       </c>
       <c r="L18" t="n">
         <v>0.07000000000000001</v>
@@ -1851,10 +1851,10 @@
         <v>272.25</v>
       </c>
       <c r="E19" t="n">
-        <v>3.969093165210287</v>
+        <v>3.969093061921526</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4540541330781472</v>
+        <v>0.4540541212621765</v>
       </c>
       <c r="G19" t="n">
         <v>-13.21</v>
@@ -1869,7 +1869,7 @@
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.2713272641984574</v>
+        <v>0.2713272712592787</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1922,10 +1922,10 @@
         <v>268.5</v>
       </c>
       <c r="E20" t="n">
-        <v>0.09996683862160764</v>
+        <v>0.09996363266789167</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2355328063017005</v>
+        <v>0.2355252527240741</v>
       </c>
       <c r="G20" t="n">
         <v>-0.332925</v>
@@ -1940,7 +1940,7 @@
         <v>-0.332925</v>
       </c>
       <c r="K20" t="n">
-        <v>1.008237108189759</v>
+        <v>1.008269443564308</v>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
@@ -2009,10 +2009,10 @@
         <v>242.44</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1141710361216055</v>
+        <v>0.114167371871854</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2428909738731678</v>
+        <v>0.2428831784355429</v>
       </c>
       <c r="G21" t="n">
         <v>-0.332925</v>
@@ -2027,7 +2027,7 @@
         <v>-0.332925</v>
       </c>
       <c r="K21" t="n">
-        <v>1.007960279600445</v>
+        <v>1.007992630508971</v>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
@@ -2092,13 +2092,13 @@
         <v>103.1</v>
       </c>
       <c r="E22" t="n">
-        <v>4.82663356524879</v>
+        <v>12.48937108880229</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4979383581562272</v>
+        <v>0.5410628137990376</v>
       </c>
       <c r="G22" t="n">
-        <v>-5.547262026446624</v>
+        <v>-13.21</v>
       </c>
       <c r="H22" t="n">
         <v>4.768759915832044</v>
@@ -2110,7 +2110,7 @@
         <v>-13.21</v>
       </c>
       <c r="K22" t="n">
-        <v>0.4148938453026494</v>
+        <v>0.3818254643828795</v>
       </c>
       <c r="L22" t="n">
         <v>0.13</v>
@@ -2165,10 +2165,10 @@
         <v>329.4</v>
       </c>
       <c r="E23" t="n">
-        <v>2.511143937823774</v>
+        <v>2.511143887422177</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3475710961842789</v>
+        <v>0.3475710892081204</v>
       </c>
       <c r="G23" t="n">
         <v>-13.21</v>
@@ -2183,7 +2183,7 @@
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1959094345967349</v>
+        <v>0.1959094385288666</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2236,13 +2236,13 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>1.465955880083579</v>
+        <v>3.96909303424228</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3345898681690729</v>
+        <v>0.3806549565258843</v>
       </c>
       <c r="G24" t="n">
-        <v>-5.550743282537491</v>
+        <v>-13.21</v>
       </c>
       <c r="H24" t="n">
         <v>1.076926979514509</v>
@@ -2254,7 +2254,7 @@
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.3086836890081579</v>
+        <v>0.2713282279411472</v>
       </c>
       <c r="L24" t="n">
         <v>0.0002</v>
@@ -2309,13 +2309,13 @@
         <v>246.3</v>
       </c>
       <c r="E25" t="n">
-        <v>1.116107188502733</v>
+        <v>2.957467015229745</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2748981209755296</v>
+        <v>0.3060784639564738</v>
       </c>
       <c r="G25" t="n">
-        <v>-5.550726324288036</v>
+        <v>-13.21</v>
       </c>
       <c r="H25" t="n">
         <v>1.32388456056834</v>
@@ -2327,7 +2327,7 @@
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.4984151211020453</v>
+        <v>0.4476413612563981</v>
       </c>
       <c r="L25" t="n">
         <v>0.003</v>
@@ -2382,10 +2382,10 @@
         <v>174.15</v>
       </c>
       <c r="E26" t="n">
-        <v>9.725652483182483</v>
+        <v>9.725652288380664</v>
       </c>
       <c r="F26" t="n">
-        <v>0.7116896956384244</v>
+        <v>0.7116896813834993</v>
       </c>
       <c r="G26" t="n">
         <v>-13.21</v>
@@ -2400,7 +2400,7 @@
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.4692139823070383</v>
+        <v>0.4692139917052498</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2453,10 +2453,10 @@
         <v>270.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1013988328992703</v>
+        <v>0.1013955785655886</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2406863074977069</v>
+        <v>0.2406785828175028</v>
       </c>
       <c r="G27" t="n">
         <v>-0.332925</v>
@@ -2471,7 +2471,7 @@
         <v>-0.332925</v>
       </c>
       <c r="K27" t="n">
-        <v>1.008369642298898</v>
+        <v>1.008402006346098</v>
       </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
@@ -2536,13 +2536,13 @@
         <v>104.15</v>
       </c>
       <c r="E28" t="n">
-        <v>2.49154978025147</v>
+        <v>6.766253948281869</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2594955561592865</v>
+        <v>0.2961120081300709</v>
       </c>
       <c r="G28" t="n">
-        <v>-5.550731080009657</v>
+        <v>-13.21</v>
       </c>
       <c r="H28" t="n">
         <v>2.989826998793612</v>
@@ -2554,7 +2554,7 @@
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.5042244029257243</v>
+        <v>0.4418733056202847</v>
       </c>
       <c r="L28" t="n">
         <v>0.001</v>
@@ -2609,10 +2609,10 @@
         <v>824.3</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1308412067177736</v>
+        <v>0.1308423118282197</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2719787484419812</v>
+        <v>0.2719810456277346</v>
       </c>
       <c r="G29" t="n">
         <v>-2.20113372715757</v>
@@ -2627,7 +2627,7 @@
         <v>-2.201133727157571</v>
       </c>
       <c r="K29" t="n">
-        <v>0.4515330409436112</v>
+        <v>0.4515292272393641</v>
       </c>
       <c r="L29" t="n">
         <v>0.14</v>
@@ -2694,10 +2694,10 @@
         <v>126.11004</v>
       </c>
       <c r="E30" t="n">
-        <v>0.007105680059812832</v>
+        <v>0.007105611207608455</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06718478315650384</v>
+        <v>0.06718413215330893</v>
       </c>
       <c r="G30" t="n">
         <v>-0.078476895921783</v>

</xml_diff>

<commit_message>
reran yields w/ pFBA
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP/compiled_results.xlsx
+++ b/application/output_max_withoutMP/compiled_results.xlsx
@@ -616,10 +616,10 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.81382230371743</v>
+        <v>17.81382266698288</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5695516989363105</v>
+        <v>0.5695517105508002</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
@@ -634,7 +634,7 @@
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5800987449892061</v>
+        <v>0.5800987331596378</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -687,10 +687,10 @@
         <v>122.16</v>
       </c>
       <c r="E3" t="n">
-        <v>6.941370125627985</v>
+        <v>6.941370261962294</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3563056245974301</v>
+        <v>0.3563056315955702</v>
       </c>
       <c r="G3" t="n">
         <v>-13.21</v>
@@ -705,7 +705,7 @@
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5425276561925623</v>
+        <v>0.5425276455368662</v>
       </c>
       <c r="L3" t="n">
         <v>0.08</v>
@@ -760,10 +760,10 @@
         <v>90.08</v>
       </c>
       <c r="E4" t="n">
-        <v>20.06614466395784</v>
+        <v>20.06614507315321</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7595227173413802</v>
+        <v>0.7595227328298153</v>
       </c>
       <c r="G4" t="n">
         <v>-13.21</v>
@@ -778,7 +778,7 @@
         <v>-13.21</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2387059012575083</v>
+        <v>0.2387058963897398</v>
       </c>
       <c r="L4" t="n">
         <v>0.13</v>
@@ -833,10 +833,10 @@
         <v>90.08</v>
       </c>
       <c r="E5" t="n">
-        <v>22.34089268642791</v>
+        <v>22.34089323932462</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8456240999550857</v>
+        <v>0.8456241208827535</v>
       </c>
       <c r="G5" t="n">
         <v>-13.21</v>
@@ -851,7 +851,7 @@
         <v>-13.21</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3703426456444216</v>
+        <v>0.3703426364791108</v>
       </c>
       <c r="L5" t="n">
         <v>0.14</v>
@@ -906,10 +906,10 @@
         <v>90.08</v>
       </c>
       <c r="E6" t="n">
-        <v>20.06614466395784</v>
+        <v>20.06614507315321</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7595227173413802</v>
+        <v>0.7595227328298153</v>
       </c>
       <c r="G6" t="n">
         <v>-13.21</v>
@@ -924,7 +924,7 @@
         <v>-13.21</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2387059012575083</v>
+        <v>0.2387058963897398</v>
       </c>
       <c r="L6" t="n">
         <v>0.13</v>
@@ -979,10 +979,10 @@
         <v>90.08</v>
       </c>
       <c r="E7" t="n">
-        <v>22.34089268642791</v>
+        <v>22.34089323932462</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8456240999550857</v>
+        <v>0.8456241208827535</v>
       </c>
       <c r="G7" t="n">
         <v>-13.21</v>
@@ -997,7 +997,7 @@
         <v>-13.21</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3703426456444216</v>
+        <v>0.3703426364791108</v>
       </c>
       <c r="L7" t="n">
         <v>0.14</v>
@@ -1052,10 +1052,10 @@
         <v>137.11</v>
       </c>
       <c r="E8" t="n">
-        <v>9.055952018579516</v>
+        <v>9.055952191748684</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5217370705618246</v>
+        <v>0.5217370805385532</v>
       </c>
       <c r="G8" t="n">
         <v>-13.21</v>
@@ -1070,7 +1070,7 @@
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>0.3535611126095911</v>
+        <v>0.3535611058487466</v>
       </c>
       <c r="L8" t="n">
         <v>0.07000000000000001</v>
@@ -1125,10 +1125,10 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.844697670245612</v>
+        <v>2.8446977520824</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2800995824094576</v>
+        <v>0.2800995904674141</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
@@ -1143,7 +1143,7 @@
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4459930778203111</v>
+        <v>0.4459930649899002</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1196,10 +1196,10 @@
         <v>90.12</v>
       </c>
       <c r="E10" t="n">
-        <v>12.89443800817266</v>
+        <v>12.89443786899621</v>
       </c>
       <c r="F10" t="n">
-        <v>0.488283504996536</v>
+        <v>0.4882834997262354</v>
       </c>
       <c r="G10" t="n">
         <v>-13.21</v>
@@ -1214,7 +1214,7 @@
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>0.9974082096827768</v>
+        <v>0.997408220448328</v>
       </c>
       <c r="L10" t="n">
         <v>0.11</v>
@@ -1269,10 +1269,10 @@
         <v>74.12</v>
       </c>
       <c r="E11" t="n">
-        <v>11.19787340381384</v>
+        <v>11.1978733226628</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3487541753033827</v>
+        <v>0.3487541727759596</v>
       </c>
       <c r="G11" t="n">
         <v>-13.21</v>
@@ -1287,7 +1287,7 @@
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7847593339747708</v>
+        <v>0.7847593396619253</v>
       </c>
       <c r="L11" t="n">
         <v>0.04</v>
@@ -1342,10 +1342,10 @@
         <v>146.1</v>
       </c>
       <c r="E12" t="n">
-        <v>12.48937108880212</v>
+        <v>12.48937153880213</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7667243171293728</v>
+        <v>0.7667243447549389</v>
       </c>
       <c r="G12" t="n">
         <v>-13.21</v>
@@ -1360,7 +1360,7 @@
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>0.3990386909380151</v>
+        <v>0.3990386765603972</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1413,10 +1413,10 @@
         <v>163.15</v>
       </c>
       <c r="E13" t="n">
-        <v>7.096204298631618</v>
+        <v>7.096204443792231</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4864762471741197</v>
+        <v>0.4864762571255229</v>
       </c>
       <c r="G13" t="n">
         <v>-13.21</v>
@@ -1431,7 +1431,7 @@
         <v>-13.21</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4351111376023918</v>
+        <v>0.4351111287017182</v>
       </c>
       <c r="L13" t="n">
         <v>0.15</v>
@@ -1486,10 +1486,10 @@
         <v>256.4</v>
       </c>
       <c r="E14" t="n">
-        <v>2.761960161636383</v>
+        <v>2.761960230576627</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2975663943648403</v>
+        <v>0.2975664017922826</v>
       </c>
       <c r="G14" t="n">
         <v>-13.21</v>
@@ -1504,7 +1504,7 @@
         <v>-13.21</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2594030857008648</v>
+        <v>0.2594030792260025</v>
       </c>
       <c r="L14" t="n">
         <v>0.1</v>
@@ -1559,10 +1559,10 @@
         <v>242.44</v>
       </c>
       <c r="E15" t="n">
-        <v>2.677177440227001</v>
+        <v>2.677177506303691</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2727280980121854</v>
+        <v>0.2727281047435173</v>
       </c>
       <c r="G15" t="n">
         <v>-13.21</v>
@@ -1577,7 +1577,7 @@
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.2720593916947378</v>
+        <v>0.2720593849799107</v>
       </c>
       <c r="L15" t="n">
         <v>0.005</v>
@@ -1632,10 +1632,10 @@
         <v>74.12</v>
       </c>
       <c r="E16" t="n">
-        <v>12.52385380260018</v>
+        <v>12.52385415259966</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3900514094987328</v>
+        <v>0.3900514203993543</v>
       </c>
       <c r="G16" t="n">
         <v>-13.21</v>
@@ -1650,7 +1650,7 @@
         <v>-13.21</v>
       </c>
       <c r="K16" t="n">
-        <v>0.9872554154549874</v>
+        <v>0.9872553878645289</v>
       </c>
       <c r="L16" t="n">
         <v>0.06</v>
@@ -1705,10 +1705,10 @@
         <v>89.06999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>24.24659146894892</v>
+        <v>24.24659196339342</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9074664948630357</v>
+        <v>0.9074665133683922</v>
       </c>
       <c r="G17" t="n">
         <v>-13.21</v>
@@ -1723,7 +1723,7 @@
         <v>-13.21</v>
       </c>
       <c r="K17" t="n">
-        <v>0.8724089016032006</v>
+        <v>0.8724088838127504</v>
       </c>
       <c r="L17" t="n">
         <v>0.6899999999999999</v>
@@ -1778,10 +1778,10 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>10.42241543739891</v>
+        <v>10.42241564706572</v>
       </c>
       <c r="F18" t="n">
-        <v>0.6135132790815938</v>
+        <v>0.6135132914235861</v>
       </c>
       <c r="G18" t="n">
         <v>-13.21</v>
@@ -1796,7 +1796,7 @@
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>0.4612522986139782</v>
+        <v>0.4612522893350067</v>
       </c>
       <c r="L18" t="n">
         <v>0.07000000000000001</v>
@@ -1851,10 +1851,10 @@
         <v>272.25</v>
       </c>
       <c r="E19" t="n">
-        <v>3.969093063101203</v>
+        <v>3.96909316610889</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4540541213971285</v>
+        <v>0.4540541331809452</v>
       </c>
       <c r="G19" t="n">
         <v>-13.21</v>
@@ -1869,7 +1869,7 @@
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.271327271178636</v>
+        <v>0.2713272641370289</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1922,10 +1922,10 @@
         <v>268.5</v>
       </c>
       <c r="E20" t="n">
-        <v>0.09996363389292853</v>
+        <v>0.09996683862160761</v>
       </c>
       <c r="F20" t="n">
-        <v>0.235525255610395</v>
+        <v>0.2355328063017005</v>
       </c>
       <c r="G20" t="n">
         <v>-0.332925</v>
@@ -1940,7 +1940,7 @@
         <v>-0.332925</v>
       </c>
       <c r="K20" t="n">
-        <v>1.008269431208142</v>
+        <v>1.008237108189759</v>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
@@ -2009,10 +2009,10 @@
         <v>242.44</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1141673758657095</v>
+        <v>0.1141710361216055</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2428831869321939</v>
+        <v>0.2428909738731678</v>
       </c>
       <c r="G21" t="n">
         <v>-0.332925</v>
@@ -2027,7 +2027,7 @@
         <v>-0.332925</v>
       </c>
       <c r="K21" t="n">
-        <v>1.00799259524691</v>
+        <v>1.007960279600445</v>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
@@ -2092,10 +2092,10 @@
         <v>103.1</v>
       </c>
       <c r="E22" t="n">
-        <v>12.48937153880215</v>
+        <v>12.48937153880213</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5410628332938695</v>
+        <v>0.5410628332938684</v>
       </c>
       <c r="G22" t="n">
         <v>-13.21</v>
@@ -2110,7 +2110,7 @@
         <v>-13.21</v>
       </c>
       <c r="K22" t="n">
-        <v>0.3818254506254695</v>
+        <v>0.3818254506254702</v>
       </c>
       <c r="L22" t="n">
         <v>0.13</v>
@@ -2165,10 +2165,10 @@
         <v>329.4</v>
       </c>
       <c r="E23" t="n">
-        <v>2.511143895123665</v>
+        <v>2.511143938761768</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3475710902740945</v>
+        <v>0.347571096314108</v>
       </c>
       <c r="G23" t="n">
         <v>-13.21</v>
@@ -2183,7 +2183,7 @@
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1959094379280272</v>
+        <v>0.1959094345235564</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2236,10 +2236,10 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>3.969093061921534</v>
+        <v>3.969093165426386</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3806549591804568</v>
+        <v>0.3806549691070659</v>
       </c>
       <c r="G24" t="n">
         <v>-13.21</v>
@@ -2254,7 +2254,7 @@
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.2713282260489863</v>
+        <v>0.2713282189733681</v>
       </c>
       <c r="L24" t="n">
         <v>0.0002</v>
@@ -2309,10 +2309,10 @@
         <v>246.3</v>
       </c>
       <c r="E25" t="n">
-        <v>2.957467113780485</v>
+        <v>2.957467099771051</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3060784741558298</v>
+        <v>0.3060784727059451</v>
       </c>
       <c r="G25" t="n">
         <v>-13.21</v>
@@ -2327,7 +2327,7 @@
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.4476413463397868</v>
+        <v>0.4476413484602507</v>
       </c>
       <c r="L25" t="n">
         <v>0.003</v>
@@ -2382,10 +2382,10 @@
         <v>174.15</v>
       </c>
       <c r="E26" t="n">
-        <v>9.725652288380617</v>
+        <v>9.725652483182481</v>
       </c>
       <c r="F26" t="n">
-        <v>0.711689681383496</v>
+        <v>0.7116896956384242</v>
       </c>
       <c r="G26" t="n">
         <v>-13.21</v>
@@ -2400,7 +2400,7 @@
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.469213991705252</v>
+        <v>0.4692139823070384</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2453,10 +2453,10 @@
         <v>270.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.101395582263834</v>
+        <v>0.1013988328992703</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2406785915958784</v>
+        <v>0.2406863074977069</v>
       </c>
       <c r="G27" t="n">
         <v>-0.332925</v>
@@ -2471,7 +2471,7 @@
         <v>-0.332925</v>
       </c>
       <c r="K27" t="n">
-        <v>1.008401969566211</v>
+        <v>1.008369642298898</v>
       </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
@@ -2536,10 +2536,10 @@
         <v>104.15</v>
       </c>
       <c r="E28" t="n">
-        <v>6.766253948281854</v>
+        <v>6.766254088154464</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2961120081300702</v>
+        <v>0.2961120142513243</v>
       </c>
       <c r="G28" t="n">
         <v>-13.21</v>
@@ -2554,7 +2554,7 @@
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.4418733056202857</v>
+        <v>0.4418732964858411</v>
       </c>
       <c r="L28" t="n">
         <v>0.001</v>
@@ -2609,10 +2609,10 @@
         <v>824.3</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1308423284963125</v>
+        <v>0.1308412072971918</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2719810802755884</v>
+        <v>0.2719787496464139</v>
       </c>
       <c r="G29" t="n">
         <v>-2.20113372715757</v>
@@ -2627,7 +2627,7 @@
         <v>-2.201133727157571</v>
       </c>
       <c r="K29" t="n">
-        <v>0.4515291697187504</v>
+        <v>0.4515330389440391</v>
       </c>
       <c r="L29" t="n">
         <v>0.14</v>
@@ -2694,10 +2694,10 @@
         <v>126.11004</v>
       </c>
       <c r="E30" t="n">
-        <v>0.007105612009973482</v>
+        <v>0.00710568005981288</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06718413973973555</v>
+        <v>0.06718478315650429</v>
       </c>
       <c r="G30" t="n">
         <v>-0.078476895921783</v>

</xml_diff>

<commit_message>
reran yields; removing stop codon ATP bug didn't change any yields significantly
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP/compiled_results.xlsx
+++ b/application/output_max_withoutMP/compiled_results.xlsx
@@ -616,25 +616,25 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.81382266698288</v>
+        <v>17.81382212023962</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5695517105508002</v>
+        <v>0.5695516930700739</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
       </c>
       <c r="H2" t="n">
-        <v>10.33377596184721</v>
+        <v>10.33594910460783</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3303962257594239</v>
+        <v>0.330465706476714</v>
       </c>
       <c r="J2" t="n">
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5800987331596378</v>
+        <v>0.5802207429063961</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -654,11 +654,11 @@
       </c>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="n">
-        <v>10.33377596184721</v>
+        <v>10.33594910460783</v>
       </c>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
-        <v>0.3303962257594239</v>
+        <v>0.330465706476714</v>
       </c>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
@@ -687,25 +687,25 @@
         <v>122.16</v>
       </c>
       <c r="E3" t="n">
-        <v>6.941370261962294</v>
+        <v>6.941370050829049</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3563056315955702</v>
+        <v>0.3563056207579458</v>
       </c>
       <c r="G3" t="n">
         <v>-13.21</v>
       </c>
       <c r="H3" t="n">
-        <v>3.765885265022023</v>
+        <v>3.766823882528126</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1933056554010707</v>
+        <v>0.1933538353267507</v>
       </c>
       <c r="J3" t="n">
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5425276455368662</v>
+        <v>0.5426628828235762</v>
       </c>
       <c r="L3" t="n">
         <v>0.08</v>
@@ -727,11 +727,11 @@
       </c>
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="n">
-        <v>3.765885265022023</v>
+        <v>3.766823882528126</v>
       </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="n">
-        <v>0.1933056554010707</v>
+        <v>0.1933538353267507</v>
       </c>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
@@ -760,25 +760,25 @@
         <v>90.08</v>
       </c>
       <c r="E4" t="n">
-        <v>20.06614507315321</v>
+        <v>20.06614445553155</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7595227328298153</v>
+        <v>0.7595227094522464</v>
       </c>
       <c r="G4" t="n">
         <v>-13.21</v>
       </c>
       <c r="H4" t="n">
-        <v>4.789907146773598</v>
+        <v>4.791077807930754</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1813025547685259</v>
+        <v>0.1813468654100596</v>
       </c>
       <c r="J4" t="n">
         <v>-13.21</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2387058963897398</v>
+        <v>0.2387642438510412</v>
       </c>
       <c r="L4" t="n">
         <v>0.13</v>
@@ -800,11 +800,11 @@
       </c>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="n">
-        <v>4.789907146773598</v>
+        <v>4.791077807930754</v>
       </c>
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="n">
-        <v>0.1813025547685259</v>
+        <v>0.1813468654100596</v>
       </c>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr"/>
@@ -833,25 +833,25 @@
         <v>90.08</v>
       </c>
       <c r="E5" t="n">
-        <v>22.34089323932462</v>
+        <v>22.3408925077748</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8456241208827535</v>
+        <v>0.8456240931928949</v>
       </c>
       <c r="G5" t="n">
         <v>-13.21</v>
       </c>
       <c r="H5" t="n">
-        <v>8.273785303549822</v>
+        <v>8.275594561880407</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3131706663980492</v>
+        <v>0.3132391485517779</v>
       </c>
       <c r="J5" t="n">
         <v>-13.21</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3703426364791108</v>
+        <v>0.3704236327622291</v>
       </c>
       <c r="L5" t="n">
         <v>0.14</v>
@@ -873,11 +873,11 @@
       </c>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="n">
-        <v>8.273785303549822</v>
+        <v>8.275594561880407</v>
       </c>
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="n">
-        <v>0.3131706663980492</v>
+        <v>0.3132391485517779</v>
       </c>
       <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="inlineStr"/>
@@ -906,25 +906,25 @@
         <v>90.08</v>
       </c>
       <c r="E6" t="n">
-        <v>20.06614507315321</v>
+        <v>20.06614445553155</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7595227328298153</v>
+        <v>0.7595227094522464</v>
       </c>
       <c r="G6" t="n">
         <v>-13.21</v>
       </c>
       <c r="H6" t="n">
-        <v>4.789907146773598</v>
+        <v>4.791077807930754</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1813025547685259</v>
+        <v>0.1813468654100596</v>
       </c>
       <c r="J6" t="n">
         <v>-13.21</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2387058963897398</v>
+        <v>0.2387642438510412</v>
       </c>
       <c r="L6" t="n">
         <v>0.13</v>
@@ -946,11 +946,11 @@
       </c>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="n">
-        <v>4.789907146773598</v>
+        <v>4.791077807930754</v>
       </c>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="n">
-        <v>0.1813025547685259</v>
+        <v>0.1813468654100596</v>
       </c>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="inlineStr"/>
@@ -979,25 +979,25 @@
         <v>90.08</v>
       </c>
       <c r="E7" t="n">
-        <v>22.34089323932462</v>
+        <v>22.3408925077748</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8456241208827535</v>
+        <v>0.8456240931928949</v>
       </c>
       <c r="G7" t="n">
         <v>-13.21</v>
       </c>
       <c r="H7" t="n">
-        <v>8.273785303549822</v>
+        <v>8.275594561880407</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3131706663980492</v>
+        <v>0.3132391485517779</v>
       </c>
       <c r="J7" t="n">
         <v>-13.21</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3703426364791108</v>
+        <v>0.3704236327622291</v>
       </c>
       <c r="L7" t="n">
         <v>0.14</v>
@@ -1019,11 +1019,11 @@
       </c>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="n">
-        <v>8.273785303549822</v>
+        <v>8.275594561880407</v>
       </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="n">
-        <v>0.3131706663980492</v>
+        <v>0.3132391485517779</v>
       </c>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
@@ -1052,25 +1052,25 @@
         <v>137.11</v>
       </c>
       <c r="E8" t="n">
-        <v>9.055952191748684</v>
+        <v>9.055951931401262</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5217370805385532</v>
+        <v>0.5217370655392575</v>
       </c>
       <c r="G8" t="n">
         <v>-13.21</v>
       </c>
       <c r="H8" t="n">
-        <v>3.201832471428046</v>
+        <v>3.202635267542847</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1844659391575074</v>
+        <v>0.1845121903404129</v>
       </c>
       <c r="J8" t="n">
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>0.3535611058487466</v>
+        <v>0.3536497644646057</v>
       </c>
       <c r="L8" t="n">
         <v>0.07000000000000001</v>
@@ -1092,11 +1092,11 @@
       </c>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="n">
-        <v>3.201832471428046</v>
+        <v>3.202635267542847</v>
       </c>
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="n">
-        <v>0.1844659391575074</v>
+        <v>0.1845121903404129</v>
       </c>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
@@ -1125,25 +1125,25 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.8446977520824</v>
+        <v>2.844697655376507</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2800995904674141</v>
+        <v>0.2800995809453898</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
       </c>
       <c r="H9" t="n">
-        <v>1.268715469421109</v>
+        <v>1.26906454502506</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1249224748549778</v>
+        <v>0.1249568461457898</v>
       </c>
       <c r="J9" t="n">
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4459930649899002</v>
+        <v>0.4461157911198456</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1163,11 +1163,11 @@
       </c>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="n">
-        <v>1.268715469421109</v>
+        <v>1.26906454502506</v>
       </c>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
-        <v>0.1249224748549778</v>
+        <v>0.1249568461457898</v>
       </c>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="inlineStr"/>
@@ -1196,25 +1196,25 @@
         <v>90.12</v>
       </c>
       <c r="E10" t="n">
-        <v>12.89443786899621</v>
+        <v>12.89443784637229</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4882834997262354</v>
+        <v>0.4882834988695184</v>
       </c>
       <c r="G10" t="n">
         <v>-13.21</v>
       </c>
       <c r="H10" t="n">
-        <v>12.86101832859704</v>
+        <v>12.86104513542536</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4870179765362261</v>
+        <v>0.4870189916508114</v>
       </c>
       <c r="J10" t="n">
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>0.997408220448328</v>
+        <v>0.9974103011434248</v>
       </c>
       <c r="L10" t="n">
         <v>0.11</v>
@@ -1236,11 +1236,11 @@
       </c>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="n">
-        <v>12.86101832859704</v>
+        <v>12.86104513542536</v>
       </c>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
-        <v>0.4870179765362261</v>
+        <v>0.4870189916508114</v>
       </c>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="inlineStr"/>
@@ -1269,25 +1269,25 @@
         <v>74.12</v>
       </c>
       <c r="E11" t="n">
-        <v>11.1978733226628</v>
+        <v>11.19787295673656</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3487541727759596</v>
+        <v>0.3487541613793045</v>
       </c>
       <c r="G11" t="n">
         <v>-13.21</v>
       </c>
       <c r="H11" t="n">
-        <v>8.787635674310746</v>
+        <v>8.788049471121706</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2736880943320031</v>
+        <v>0.2737009819009499</v>
       </c>
       <c r="J11" t="n">
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7847593396619253</v>
+        <v>0.7847963184682207</v>
       </c>
       <c r="L11" t="n">
         <v>0.04</v>
@@ -1309,11 +1309,11 @@
       </c>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="n">
-        <v>8.787635674310746</v>
+        <v>8.788049471121706</v>
       </c>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
-        <v>0.2736880943320031</v>
+        <v>0.2737009819009499</v>
       </c>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="inlineStr"/>
@@ -1342,25 +1342,25 @@
         <v>146.1</v>
       </c>
       <c r="E12" t="n">
-        <v>12.48937153880213</v>
+        <v>12.48937108880216</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7667243447549389</v>
+        <v>0.7667243171293748</v>
       </c>
       <c r="G12" t="n">
         <v>-13.21</v>
       </c>
       <c r="H12" t="n">
-        <v>4.983742289914693</v>
+        <v>4.98485860343459</v>
       </c>
       <c r="I12" t="n">
-        <v>0.3059526678176485</v>
+        <v>0.3060211984678438</v>
       </c>
       <c r="J12" t="n">
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>0.3990386765603972</v>
+        <v>0.3991280720214939</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1380,11 +1380,11 @@
       </c>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="n">
-        <v>4.983742289914693</v>
+        <v>4.98485860343459</v>
       </c>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
-        <v>0.3059526678176485</v>
+        <v>0.3060211984678438</v>
       </c>
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="inlineStr"/>
@@ -1413,25 +1413,25 @@
         <v>163.15</v>
       </c>
       <c r="E13" t="n">
-        <v>7.096204443792231</v>
+        <v>7.0962042261573</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4864762571255229</v>
+        <v>0.4864762422056842</v>
       </c>
       <c r="G13" t="n">
         <v>-13.21</v>
       </c>
       <c r="H13" t="n">
-        <v>3.087637525036586</v>
+        <v>3.088405909928811</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2116712333244736</v>
+        <v>0.2117239095134648</v>
       </c>
       <c r="J13" t="n">
         <v>-13.21</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4351111287017182</v>
+        <v>0.4352194231593061</v>
       </c>
       <c r="L13" t="n">
         <v>0.15</v>
@@ -1453,11 +1453,11 @@
       </c>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="n">
-        <v>3.087637525036586</v>
+        <v>3.088405909928811</v>
       </c>
       <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="n">
-        <v>0.2116712333244736</v>
+        <v>0.2117239095134648</v>
       </c>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="inlineStr"/>
@@ -1486,25 +1486,25 @@
         <v>256.4</v>
       </c>
       <c r="E14" t="n">
-        <v>2.761960230576627</v>
+        <v>2.76196014032085</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2975664017922826</v>
+        <v>0.2975663920683603</v>
       </c>
       <c r="G14" t="n">
         <v>-13.21</v>
       </c>
       <c r="H14" t="n">
-        <v>0.716460988511337</v>
+        <v>0.716647387847187</v>
       </c>
       <c r="I14" t="n">
-        <v>0.07718964089911999</v>
+        <v>0.07720972307809248</v>
       </c>
       <c r="J14" t="n">
         <v>-13.21</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2594030792260025</v>
+        <v>0.2594705757643323</v>
       </c>
       <c r="L14" t="n">
         <v>0.1</v>
@@ -1526,11 +1526,11 @@
       </c>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="n">
-        <v>0.716460988511337</v>
+        <v>0.716647387847187</v>
       </c>
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="n">
-        <v>0.07718964089911999</v>
+        <v>0.07720972307809248</v>
       </c>
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="inlineStr"/>
@@ -1559,25 +1559,25 @@
         <v>242.44</v>
       </c>
       <c r="E15" t="n">
-        <v>2.677177506303691</v>
+        <v>2.677177418561634</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2727281047435173</v>
+        <v>0.2727280958051019</v>
       </c>
       <c r="G15" t="n">
         <v>-13.21</v>
       </c>
       <c r="H15" t="n">
-        <v>0.728351265847033</v>
+        <v>0.728545066263168</v>
       </c>
       <c r="I15" t="n">
-        <v>0.07419824044325798</v>
+        <v>0.0742179831835382</v>
       </c>
       <c r="J15" t="n">
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.2720593849799107</v>
+        <v>0.2721317837256348</v>
       </c>
       <c r="L15" t="n">
         <v>0.005</v>
@@ -1599,11 +1599,11 @@
       </c>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="n">
-        <v>0.728351265847033</v>
+        <v>0.728545066263168</v>
       </c>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="n">
-        <v>0.07419824044325798</v>
+        <v>0.0742179831835382</v>
       </c>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
@@ -1632,25 +1632,25 @@
         <v>74.12</v>
       </c>
       <c r="E16" t="n">
-        <v>12.52385415259966</v>
+        <v>12.52385380260014</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3900514203993543</v>
+        <v>0.3900514094987315</v>
       </c>
       <c r="G16" t="n">
         <v>-13.21</v>
       </c>
       <c r="H16" t="n">
-        <v>12.36424248898357</v>
+        <v>12.36449516216495</v>
       </c>
       <c r="I16" t="n">
-        <v>0.3850803663334749</v>
+        <v>0.385088235758661</v>
       </c>
       <c r="J16" t="n">
         <v>-13.21</v>
       </c>
       <c r="K16" t="n">
-        <v>0.9872553878645289</v>
+        <v>0.987275590808789</v>
       </c>
       <c r="L16" t="n">
         <v>0.06</v>
@@ -1672,11 +1672,11 @@
       </c>
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="n">
-        <v>12.36424248898357</v>
+        <v>12.36449516216495</v>
       </c>
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="n">
-        <v>0.3850803663334749</v>
+        <v>0.385088235758661</v>
       </c>
       <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="inlineStr"/>
@@ -1705,25 +1705,25 @@
         <v>89.06999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>24.24659196339342</v>
+        <v>24.24659121710067</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9074665133683922</v>
+        <v>0.9074664854372223</v>
       </c>
       <c r="G17" t="n">
         <v>-13.21</v>
       </c>
       <c r="H17" t="n">
-        <v>21.15294223104726</v>
+        <v>21.15780961872868</v>
       </c>
       <c r="I17" t="n">
-        <v>0.7916818480251674</v>
+        <v>0.7918640175991489</v>
       </c>
       <c r="J17" t="n">
         <v>-13.21</v>
       </c>
       <c r="K17" t="n">
-        <v>0.8724088838127504</v>
+        <v>0.8726096559010932</v>
       </c>
       <c r="L17" t="n">
         <v>0.6899999999999999</v>
@@ -1745,11 +1745,11 @@
       </c>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="n">
-        <v>21.15294223104726</v>
+        <v>21.15780961872868</v>
       </c>
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="n">
-        <v>0.7916818480251674</v>
+        <v>0.7918640175991489</v>
       </c>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
@@ -1778,25 +1778,25 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>10.42241564706572</v>
+        <v>10.42241533005079</v>
       </c>
       <c r="F18" t="n">
-        <v>0.6135132914235861</v>
+        <v>0.613513272762569</v>
       </c>
       <c r="G18" t="n">
         <v>-13.21</v>
       </c>
       <c r="H18" t="n">
-        <v>4.807363077610059</v>
+        <v>4.808491230001707</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2829844102065842</v>
+        <v>0.2830508186583736</v>
       </c>
       <c r="J18" t="n">
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>0.4612522893350067</v>
+        <v>0.4613605462581652</v>
       </c>
       <c r="L18" t="n">
         <v>0.07000000000000001</v>
@@ -1818,11 +1818,11 @@
       </c>
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="n">
-        <v>4.807363077610059</v>
+        <v>4.808491230001707</v>
       </c>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="n">
-        <v>0.2829844102065842</v>
+        <v>0.2830508186583736</v>
       </c>
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="inlineStr"/>
@@ -1851,25 +1851,25 @@
         <v>272.25</v>
       </c>
       <c r="E19" t="n">
-        <v>3.96909316610889</v>
+        <v>3.969093036182524</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4540541331809452</v>
+        <v>0.4540541183177003</v>
       </c>
       <c r="G19" t="n">
         <v>-13.21</v>
       </c>
       <c r="H19" t="n">
-        <v>1.076923189865303</v>
+        <v>1.077155928499726</v>
       </c>
       <c r="I19" t="n">
-        <v>0.123197265726096</v>
+        <v>0.1232238904321656</v>
       </c>
       <c r="J19" t="n">
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.2713272641370289</v>
+        <v>0.2713859107560088</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1889,11 +1889,11 @@
       </c>
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="n">
-        <v>1.076923189865303</v>
+        <v>1.077155928499726</v>
       </c>
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="n">
-        <v>0.123197265726096</v>
+        <v>0.1232238904321656</v>
       </c>
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="inlineStr"/>
@@ -1922,25 +1922,25 @@
         <v>268.5</v>
       </c>
       <c r="E20" t="n">
-        <v>0.09996683862160761</v>
+        <v>0.09996364001457181</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2355328063017005</v>
+        <v>0.2355252700336561</v>
       </c>
       <c r="G20" t="n">
         <v>-0.332925</v>
       </c>
       <c r="H20" t="n">
-        <v>0.100790276286722</v>
+        <v>0.100792269927017</v>
       </c>
       <c r="I20" t="n">
-        <v>0.2374729155094452</v>
+        <v>0.2374776127440473</v>
       </c>
       <c r="J20" t="n">
         <v>-0.332925</v>
       </c>
       <c r="K20" t="n">
-        <v>1.008237108189759</v>
+        <v>1.008289313117494</v>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
@@ -1968,11 +1968,11 @@
       </c>
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="n">
-        <v>0.100790276286722</v>
+        <v>0.100792269927017</v>
       </c>
       <c r="Z20" t="inlineStr"/>
       <c r="AA20" t="n">
-        <v>0.2374729155094452</v>
+        <v>0.2374776127440473</v>
       </c>
       <c r="AB20" t="inlineStr"/>
       <c r="AC20" t="n">
@@ -2009,25 +2009,25 @@
         <v>242.44</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1141710361216055</v>
+        <v>0.1141673836281253</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2428909738731678</v>
+        <v>0.242883203446196</v>
       </c>
       <c r="G21" t="n">
         <v>-0.332925</v>
       </c>
       <c r="H21" t="n">
-        <v>0.115079869491406</v>
+        <v>0.115082140347757</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2448244539376226</v>
+        <v>0.2448292850272698</v>
       </c>
       <c r="J21" t="n">
         <v>-0.332925</v>
       </c>
       <c r="K21" t="n">
-        <v>1.007960279600445</v>
+        <v>1.008012417299597</v>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
@@ -2051,11 +2051,11 @@
       </c>
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="n">
-        <v>0.115079869491406</v>
+        <v>0.115082140347757</v>
       </c>
       <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="n">
-        <v>0.2448244539376226</v>
+        <v>0.2448292850272698</v>
       </c>
       <c r="AB21" t="inlineStr"/>
       <c r="AC21" t="n">
@@ -2092,25 +2092,25 @@
         <v>103.1</v>
       </c>
       <c r="E22" t="n">
-        <v>12.48937153880213</v>
+        <v>12.48937108880215</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5410628332938684</v>
+        <v>0.5410628137990313</v>
       </c>
       <c r="G22" t="n">
         <v>-13.21</v>
       </c>
       <c r="H22" t="n">
-        <v>4.768759915832044</v>
+        <v>4.769949252897912</v>
       </c>
       <c r="I22" t="n">
-        <v>0.206591560139125</v>
+        <v>0.2066430844356519</v>
       </c>
       <c r="J22" t="n">
         <v>-13.21</v>
       </c>
       <c r="K22" t="n">
-        <v>0.3818254506254702</v>
+        <v>0.3819206923216978</v>
       </c>
       <c r="L22" t="n">
         <v>0.13</v>
@@ -2132,11 +2132,11 @@
       </c>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="n">
-        <v>4.768759915832044</v>
+        <v>4.769949252897912</v>
       </c>
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="n">
-        <v>0.206591560139125</v>
+        <v>0.2066430844356519</v>
       </c>
       <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="inlineStr"/>
@@ -2165,25 +2165,25 @@
         <v>329.4</v>
       </c>
       <c r="E23" t="n">
-        <v>2.511143938761768</v>
+        <v>2.511143874209327</v>
       </c>
       <c r="F23" t="n">
-        <v>0.347571096314108</v>
+        <v>0.3475710873793104</v>
       </c>
       <c r="G23" t="n">
         <v>-13.21</v>
       </c>
       <c r="H23" t="n">
-        <v>0.491956789050074</v>
+        <v>0.492166192311695</v>
       </c>
       <c r="I23" t="n">
-        <v>0.06809245693562944</v>
+        <v>0.06812144074658903</v>
       </c>
       <c r="J23" t="n">
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1959094345235564</v>
+        <v>0.1959928291510822</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2203,11 +2203,11 @@
       </c>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="n">
-        <v>0.491956789050074</v>
+        <v>0.492166192311695</v>
       </c>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="n">
-        <v>0.06809245693562944</v>
+        <v>0.06812144074658903</v>
       </c>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
@@ -2236,25 +2236,25 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>3.969093165426386</v>
+        <v>3.969093035873841</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3806549691070659</v>
+        <v>0.3806549566823588</v>
       </c>
       <c r="G24" t="n">
         <v>-13.21</v>
       </c>
       <c r="H24" t="n">
-        <v>1.076926979514509</v>
+        <v>1.077170959236482</v>
       </c>
       <c r="I24" t="n">
-        <v>0.1032824348111826</v>
+        <v>0.1033058336304241</v>
       </c>
       <c r="J24" t="n">
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.2713282189733681</v>
+        <v>0.2713896977220466</v>
       </c>
       <c r="L24" t="n">
         <v>0.0002</v>
@@ -2276,11 +2276,11 @@
       </c>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="n">
-        <v>1.076926979514509</v>
+        <v>1.077170959236482</v>
       </c>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="n">
-        <v>0.1032824348111826</v>
+        <v>0.1033058336304241</v>
       </c>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="inlineStr"/>
@@ -2309,25 +2309,25 @@
         <v>246.3</v>
       </c>
       <c r="E25" t="n">
-        <v>2.957467099771051</v>
+        <v>2.957466999770999</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3060784727059451</v>
+        <v>0.3060784623565949</v>
       </c>
       <c r="G25" t="n">
         <v>-13.21</v>
       </c>
       <c r="H25" t="n">
-        <v>1.32388456056834</v>
+        <v>1.324232449482202</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1370133802567433</v>
+        <v>0.137049384480572</v>
       </c>
       <c r="J25" t="n">
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.4476413484602507</v>
+        <v>0.4477589942963823</v>
       </c>
       <c r="L25" t="n">
         <v>0.003</v>
@@ -2349,11 +2349,11 @@
       </c>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="n">
-        <v>1.32388456056834</v>
+        <v>1.324232449482202</v>
       </c>
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="n">
-        <v>0.1370133802567433</v>
+        <v>0.137049384480572</v>
       </c>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="inlineStr"/>
@@ -2382,25 +2382,25 @@
         <v>174.15</v>
       </c>
       <c r="E26" t="n">
-        <v>9.725652483182481</v>
+        <v>9.725652187360838</v>
       </c>
       <c r="F26" t="n">
-        <v>0.7116896956384242</v>
+        <v>0.7116896739912171</v>
       </c>
       <c r="G26" t="n">
         <v>-13.21</v>
       </c>
       <c r="H26" t="n">
-        <v>4.563412132168388</v>
+        <v>4.564520517187828</v>
       </c>
       <c r="I26" t="n">
-        <v>0.3339347562573891</v>
+        <v>0.3340158640492313</v>
       </c>
       <c r="J26" t="n">
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.4692139823070384</v>
+        <v>0.4693279616887533</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2420,11 +2420,11 @@
       </c>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="n">
-        <v>4.563412132168388</v>
+        <v>4.564520517187828</v>
       </c>
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="n">
-        <v>0.3339347562573891</v>
+        <v>0.3340158640492313</v>
       </c>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="inlineStr"/>
@@ -2453,25 +2453,25 @@
         <v>270.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1013988328992703</v>
+        <v>0.1013955884731691</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2406863074977069</v>
+        <v>0.2406786063347258</v>
       </c>
       <c r="G27" t="n">
         <v>-0.332925</v>
       </c>
       <c r="H27" t="n">
-        <v>0.102247504860163</v>
+        <v>0.102250323106358</v>
       </c>
       <c r="I27" t="n">
-        <v>0.2427007657977054</v>
+        <v>0.2427074553546845</v>
       </c>
       <c r="J27" t="n">
         <v>-0.332925</v>
       </c>
       <c r="K27" t="n">
-        <v>1.008369642298898</v>
+        <v>1.00842970237719</v>
       </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
@@ -2495,11 +2495,11 @@
       </c>
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="n">
-        <v>0.102247504860163</v>
+        <v>0.102250323106358</v>
       </c>
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="n">
-        <v>0.2427007657977054</v>
+        <v>0.2427074553546845</v>
       </c>
       <c r="AB27" t="inlineStr"/>
       <c r="AC27" t="n">
@@ -2536,25 +2536,25 @@
         <v>104.15</v>
       </c>
       <c r="E28" t="n">
-        <v>6.766254088154464</v>
+        <v>6.76625387898346</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2961120142513243</v>
+        <v>0.2961120050973601</v>
       </c>
       <c r="G28" t="n">
         <v>-13.21</v>
       </c>
       <c r="H28" t="n">
-        <v>2.989826998793612</v>
+        <v>2.990606801680859</v>
       </c>
       <c r="I28" t="n">
-        <v>0.130843991866295</v>
+        <v>0.1308781184303663</v>
       </c>
       <c r="J28" t="n">
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.4418732964858411</v>
+        <v>0.441988558982383</v>
       </c>
       <c r="L28" t="n">
         <v>0.001</v>
@@ -2576,11 +2576,11 @@
       </c>
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="n">
-        <v>2.989826998793612</v>
+        <v>2.990606801680859</v>
       </c>
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="n">
-        <v>0.130843991866295</v>
+        <v>0.1308781184303663</v>
       </c>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="inlineStr"/>
@@ -2609,25 +2609,25 @@
         <v>824.3</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1308412072971918</v>
+        <v>0.1308423337167816</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2719787496464139</v>
+        <v>0.2719810911273429</v>
       </c>
       <c r="G29" t="n">
         <v>-2.20113372715757</v>
       </c>
       <c r="H29" t="n">
-        <v>0.059079127950008</v>
+        <v>0.059085188168694</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1228073913560453</v>
+        <v>0.1228199886924261</v>
       </c>
       <c r="J29" t="n">
         <v>-2.201133727157571</v>
       </c>
       <c r="K29" t="n">
-        <v>0.4515330389440391</v>
+        <v>0.4515754686597724</v>
       </c>
       <c r="L29" t="n">
         <v>0.14</v>
@@ -2653,11 +2653,11 @@
       </c>
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="n">
-        <v>0.059079127950008</v>
+        <v>0.059085188168694</v>
       </c>
       <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="n">
-        <v>0.1228073913560453</v>
+        <v>0.1228199886924261</v>
       </c>
       <c r="AB29" t="inlineStr"/>
       <c r="AC29" t="n">
@@ -2694,10 +2694,10 @@
         <v>126.11004</v>
       </c>
       <c r="E30" t="n">
-        <v>0.00710568005981288</v>
+        <v>0.007105612999394498</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06718478315650429</v>
+        <v>0.06718414909479177</v>
       </c>
       <c r="G30" t="n">
         <v>-0.078476895921783</v>

</xml_diff>

<commit_message>
yield rerun w/ RBA version of biomass in GSM
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP/compiled_results.xlsx
+++ b/application/output_max_withoutMP/compiled_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -616,10 +616,10 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.81382212023962</v>
+        <v>17.83579802019262</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5695516930700739</v>
+        <v>0.5702543166250014</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
@@ -634,7 +634,7 @@
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5802207429063961</v>
+        <v>0.5795058394867494</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -687,10 +687,10 @@
         <v>122.16</v>
       </c>
       <c r="E3" t="n">
-        <v>6.941370050829049</v>
+        <v>6.949933224568027</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3563056207579458</v>
+        <v>0.3567451747526734</v>
       </c>
       <c r="G3" t="n">
         <v>-13.21</v>
@@ -705,7 +705,7 @@
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5426628828235762</v>
+        <v>0.541994255313475</v>
       </c>
       <c r="L3" t="n">
         <v>0.08</v>
@@ -760,10 +760,10 @@
         <v>90.08</v>
       </c>
       <c r="E4" t="n">
-        <v>20.06614445553155</v>
+        <v>20.0908989192975</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7595227094522464</v>
+        <v>0.7604596895199529</v>
       </c>
       <c r="G4" t="n">
         <v>-13.21</v>
@@ -778,7 +778,7 @@
         <v>-13.21</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2387642438510412</v>
+        <v>0.2384700568738055</v>
       </c>
       <c r="L4" t="n">
         <v>0.13</v>
@@ -833,10 +833,10 @@
         <v>90.08</v>
       </c>
       <c r="E5" t="n">
-        <v>22.3408925077748</v>
+        <v>22.36722787308386</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8456240931928949</v>
+        <v>0.8466209118920863</v>
       </c>
       <c r="G5" t="n">
         <v>-13.21</v>
@@ -851,7 +851,7 @@
         <v>-13.21</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3704236327622291</v>
+        <v>0.369987492810365</v>
       </c>
       <c r="L5" t="n">
         <v>0.14</v>
@@ -906,10 +906,10 @@
         <v>90.08</v>
       </c>
       <c r="E6" t="n">
-        <v>20.06614445553155</v>
+        <v>20.0908989192975</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7595227094522464</v>
+        <v>0.7604596895199529</v>
       </c>
       <c r="G6" t="n">
         <v>-13.21</v>
@@ -924,7 +924,7 @@
         <v>-13.21</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2387642438510412</v>
+        <v>0.2384700568738055</v>
       </c>
       <c r="L6" t="n">
         <v>0.13</v>
@@ -979,10 +979,10 @@
         <v>90.08</v>
       </c>
       <c r="E7" t="n">
-        <v>22.3408925077748</v>
+        <v>22.36722787308386</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8456240931928949</v>
+        <v>0.8466209118920863</v>
       </c>
       <c r="G7" t="n">
         <v>-13.21</v>
@@ -997,7 +997,7 @@
         <v>-13.21</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3704236327622291</v>
+        <v>0.369987492810365</v>
       </c>
       <c r="L7" t="n">
         <v>0.14</v>
@@ -1052,10 +1052,10 @@
         <v>137.11</v>
       </c>
       <c r="E8" t="n">
-        <v>9.055951931401262</v>
+        <v>9.067515113986417</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5217370655392575</v>
+        <v>0.5224032507173562</v>
       </c>
       <c r="G8" t="n">
         <v>-13.21</v>
@@ -1070,7 +1070,7 @@
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>0.3536497644646057</v>
+        <v>0.3531987790792718</v>
       </c>
       <c r="L8" t="n">
         <v>0.07000000000000001</v>
@@ -1125,10 +1125,10 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.844697655376507</v>
+        <v>2.848304889328497</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2800995809453898</v>
+        <v>0.2804547627048343</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
@@ -1143,7 +1143,7 @@
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4461157911198456</v>
+        <v>0.4455508080542069</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1196,10 +1196,10 @@
         <v>90.12</v>
       </c>
       <c r="E10" t="n">
-        <v>12.89443784637229</v>
+        <v>12.93506843424415</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4882834988695184</v>
+        <v>0.48982208828641</v>
       </c>
       <c r="G10" t="n">
         <v>-13.21</v>
@@ -1214,7 +1214,7 @@
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>0.9974103011434248</v>
+        <v>0.994277316800055</v>
       </c>
       <c r="L10" t="n">
         <v>0.11</v>
@@ -1269,10 +1269,10 @@
         <v>74.12</v>
       </c>
       <c r="E11" t="n">
-        <v>11.19787295673656</v>
+        <v>11.21102148593617</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3487541613793045</v>
+        <v>0.3491636681036706</v>
       </c>
       <c r="G11" t="n">
         <v>-13.21</v>
@@ -1287,7 +1287,7 @@
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7847963184682207</v>
+        <v>0.7838758923213196</v>
       </c>
       <c r="L11" t="n">
         <v>0.04</v>
@@ -1342,10 +1342,10 @@
         <v>146.1</v>
       </c>
       <c r="E12" t="n">
-        <v>12.48937108880216</v>
+        <v>12.50281531047952</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7667243171293748</v>
+        <v>0.7675496598637382</v>
       </c>
       <c r="G12" t="n">
         <v>-13.21</v>
@@ -1360,7 +1360,7 @@
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>0.3991280720214939</v>
+        <v>0.398698891381401</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1413,10 +1413,10 @@
         <v>163.15</v>
       </c>
       <c r="E13" t="n">
-        <v>7.0962042261573</v>
+        <v>7.104774546832009</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4864762422056842</v>
+        <v>0.4870637756620864</v>
       </c>
       <c r="G13" t="n">
         <v>-13.21</v>
@@ -1431,7 +1431,7 @@
         <v>-13.21</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4352194231593061</v>
+        <v>0.434694428313129</v>
       </c>
       <c r="L13" t="n">
         <v>0.15</v>
@@ -1486,10 +1486,10 @@
         <v>256.4</v>
       </c>
       <c r="E14" t="n">
-        <v>2.76196014032085</v>
+        <v>2.765203229139217</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2975663920683603</v>
+        <v>0.2979157940111148</v>
       </c>
       <c r="G14" t="n">
         <v>-13.21</v>
@@ -1504,7 +1504,7 @@
         <v>-13.21</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2594705757643323</v>
+        <v>0.2591662631864758</v>
       </c>
       <c r="L14" t="n">
         <v>0.1</v>
@@ -1559,10 +1559,10 @@
         <v>242.44</v>
       </c>
       <c r="E15" t="n">
-        <v>2.677177418561634</v>
+        <v>2.680320957381447</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2727280958051019</v>
+        <v>0.2730483328392531</v>
       </c>
       <c r="G15" t="n">
         <v>-13.21</v>
@@ -1577,7 +1577,7 @@
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.2721317837256348</v>
+        <v>0.2718126216402545</v>
       </c>
       <c r="L15" t="n">
         <v>0.005</v>
@@ -1632,10 +1632,10 @@
         <v>74.12</v>
       </c>
       <c r="E16" t="n">
-        <v>12.52385380260014</v>
+        <v>12.54392383586099</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3900514094987315</v>
+        <v>0.3906764842469256</v>
       </c>
       <c r="G16" t="n">
         <v>-13.21</v>
@@ -1650,7 +1650,7 @@
         <v>-13.21</v>
       </c>
       <c r="K16" t="n">
-        <v>0.987275590808789</v>
+        <v>0.9856959691366205</v>
       </c>
       <c r="L16" t="n">
         <v>0.06</v>
@@ -1705,10 +1705,10 @@
         <v>89.06999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>24.24659121710067</v>
+        <v>24.27650286081777</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9074664854372223</v>
+        <v>0.9085859753463218</v>
       </c>
       <c r="G17" t="n">
         <v>-13.21</v>
@@ -1723,7 +1723,7 @@
         <v>-13.21</v>
       </c>
       <c r="K17" t="n">
-        <v>0.8726096559010932</v>
+        <v>0.8715344932517999</v>
       </c>
       <c r="L17" t="n">
         <v>0.6899999999999999</v>
@@ -1778,10 +1778,10 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>10.42241533005079</v>
+        <v>10.43527287151567</v>
       </c>
       <c r="F18" t="n">
-        <v>0.613513272762569</v>
+        <v>0.6142701292199257</v>
       </c>
       <c r="G18" t="n">
         <v>-13.21</v>
@@ -1796,7 +1796,7 @@
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>0.4613605462581652</v>
+        <v>0.4607920932405188</v>
       </c>
       <c r="L18" t="n">
         <v>0.07000000000000001</v>
@@ -1851,10 +1851,10 @@
         <v>272.25</v>
       </c>
       <c r="E19" t="n">
-        <v>3.969093036182524</v>
+        <v>3.974395028628913</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4540541183177003</v>
+        <v>0.4546606527283644</v>
       </c>
       <c r="G19" t="n">
         <v>-13.21</v>
@@ -1869,7 +1869,7 @@
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.2713859107560088</v>
+        <v>0.2710238717441542</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1922,10 +1922,10 @@
         <v>268.5</v>
       </c>
       <c r="E20" t="n">
-        <v>0.09996364001457181</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2355252700336561</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
         <v>-0.332925</v>
@@ -1939,8 +1939,10 @@
       <c r="J20" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="K20" t="n">
-        <v>1.008289313117494</v>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
@@ -2009,13 +2011,13 @@
         <v>242.44</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1141673836281253</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.242883203446196</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.332925</v>
+        <v>-0.2904283587044502</v>
       </c>
       <c r="H21" t="n">
         <v>0.115082140347757</v>
@@ -2026,8 +2028,10 @@
       <c r="J21" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="K21" t="n">
-        <v>1.008012417299597</v>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
@@ -2092,10 +2096,10 @@
         <v>103.1</v>
       </c>
       <c r="E22" t="n">
-        <v>12.48937108880215</v>
+        <v>12.50281576818371</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5410628137990313</v>
+        <v>0.541645262347088</v>
       </c>
       <c r="G22" t="n">
         <v>-13.21</v>
@@ -2110,7 +2114,7 @@
         <v>-13.21</v>
       </c>
       <c r="K22" t="n">
-        <v>0.3819206923216978</v>
+        <v>0.3815100007340863</v>
       </c>
       <c r="L22" t="n">
         <v>0.13</v>
@@ -2165,10 +2169,10 @@
         <v>329.4</v>
       </c>
       <c r="E23" t="n">
-        <v>2.511143874209327</v>
+        <v>2.516212267075455</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3475710873793104</v>
+        <v>0.3482726110306784</v>
       </c>
       <c r="G23" t="n">
         <v>-13.21</v>
@@ -2183,7 +2187,7 @@
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1959928291510822</v>
+        <v>0.1955980418471334</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2236,10 +2240,10 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>3.969093035873841</v>
+        <v>3.974395028628931</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3806549566823588</v>
+        <v>0.3811634430807067</v>
       </c>
       <c r="G24" t="n">
         <v>-13.21</v>
@@ -2254,7 +2258,7 @@
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.2713896977220466</v>
+        <v>0.2710276536371574</v>
       </c>
       <c r="L24" t="n">
         <v>0.0002</v>
@@ -2309,10 +2313,10 @@
         <v>246.3</v>
       </c>
       <c r="E25" t="n">
-        <v>2.957466999770999</v>
+        <v>2.961217231488562</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3060784623565949</v>
+        <v>0.3064665867744434</v>
       </c>
       <c r="G25" t="n">
         <v>-13.21</v>
@@ -2327,7 +2331,7 @@
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.4477589942963823</v>
+        <v>0.4471919301970728</v>
       </c>
       <c r="L25" t="n">
         <v>0.003</v>
@@ -2382,10 +2386,10 @@
         <v>174.15</v>
       </c>
       <c r="E26" t="n">
-        <v>9.725652187360838</v>
+        <v>9.737650172584237</v>
       </c>
       <c r="F26" t="n">
-        <v>0.7116896739912171</v>
+        <v>0.7125676451573347</v>
       </c>
       <c r="G26" t="n">
         <v>-13.21</v>
@@ -2400,7 +2404,7 @@
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.4693279616887533</v>
+        <v>0.4687496917930938</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2453,10 +2457,10 @@
         <v>270.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1013955884731691</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2406786063347258</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
         <v>-0.332925</v>
@@ -2470,8 +2474,10 @@
       <c r="J27" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="K27" t="n">
-        <v>1.00842970237719</v>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
@@ -2536,10 +2542,10 @@
         <v>104.15</v>
       </c>
       <c r="E28" t="n">
-        <v>6.76625387898346</v>
+        <v>6.774435839264163</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2961120050973601</v>
+        <v>0.2964700727530642</v>
       </c>
       <c r="G28" t="n">
         <v>-13.21</v>
@@ -2554,7 +2560,7 @@
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.441988558982383</v>
+        <v>0.441454738466561</v>
       </c>
       <c r="L28" t="n">
         <v>0.001</v>
@@ -2609,10 +2615,10 @@
         <v>824.3</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1308423337167816</v>
+        <v>0.1333366471518599</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2719810911273429</v>
+        <v>0.2771660039182953</v>
       </c>
       <c r="G29" t="n">
         <v>-2.20113372715757</v>
@@ -2627,7 +2633,7 @@
         <v>-2.201133727157571</v>
       </c>
       <c r="K29" t="n">
-        <v>0.4515754686597724</v>
+        <v>0.4431278979244214</v>
       </c>
       <c r="L29" t="n">
         <v>0.14</v>
@@ -2635,7 +2641,7 @@
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr">
         <is>
-          <t>c_sources:EX_glc__D_e;BIOMASS_AERO_SC_hvd:(0.009615384615,0.14);EX_glc__D_e:(-2.20113372715757,1000);EX_nh4_e:(-0.181824845165991,1000);EX_o2_e:(-26.25403530509562,1000)</t>
+          <t>c_sources:EX_glc__D_e;BIOMASS_AERO_SC_RBA:(0.009615384615,0.14);EX_glc__D_e:(-2.20113372715757,1000);EX_nh4_e:(-0.181824845165991,1000);EX_o2_e:(-26.25403530509562,1000)</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
@@ -2694,10 +2700,10 @@
         <v>126.11004</v>
       </c>
       <c r="E30" t="n">
-        <v>0.007105612999394498</v>
+        <v>-8.946889123367239e-07</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06718414909479177</v>
+        <v>8.45935646720553e-06</v>
       </c>
       <c r="G30" t="n">
         <v>-0.078476895921783</v>
@@ -2710,7 +2716,7 @@
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr">
         <is>
-          <t>c_sources:EX_xyl__D_e,EX_glc__D_e;EX_xyl__D_e:(-0.0266525306904169,-0.0266525306904169);EX_glc__D_e:(-0.0518243652313661,-0.0518243652313661);BIOMASS_AERO_SC_hvd:(0,0.0138888888888889);BiomassKim_e:(0,0);EX_btn_c:(0,0.02);ATPM_c:(0,1000);EX_4abz_e:(-1000,1000);EX_fe3_e:(-1000,1000);EX_fol_e:(-1000,1000);EX_inost_e:(-1000,1000);EX_nac_e:(-1000,1000);EX_pnto__R_e:(-1000,1000);EX_pydxn_e:(-1000,1000);EX_ribflv_e:(-1000,1000);EX_thm_e:(-1000,1000);EX_o2_e:(-26.25403530509562,1000)</t>
+          <t>c_sources:EX_xyl__D_e,EX_glc__D_e;EX_xyl__D_e:(-0.0266525306904169,-0.0266525306904169);EX_glc__D_e:(-0.0518243652313661,-0.0518243652313661);BIOMASS_AERO_SC_RBA:(0.0138888888888888,0.0138888888888889);ATPM_c:(0,1000);EX_4abz_e:(-1000,1000);EX_fe3_e:(-1000,1000);EX_fol_e:(-1000,1000);EX_inost_e:(-1000,1000);EX_nac_e:(-1000,1000);EX_pnto__R_e:(-1000,1000);EX_pydxn_e:(-1000,1000);EX_ribflv_e:(-1000,1000);EX_thm_e:(-1000,1000);EX_o2_e:(-26.25403530509562,1000)</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>

</xml_diff>